<commit_message>
* Changed radix of CPU algorithms to 16 * Rerun radix sort benchmarks * Wrote radix sort CPU chapter
</commit_message>
<xml_diff>
--- a/latex/charts/2013_08_15_sort_high_res.xlsx
+++ b/latex/charts/2013_08_15_sort_high_res.xlsx
@@ -570,7 +570,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2591,367 +2592,367 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="121"/>
                 <c:pt idx="0">
-                  <c:v>3.0000000000000001E-6</c:v>
+                  <c:v>5.7799999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999999995E-7</c:v>
+                  <c:v>5.5999999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0000000000000001E-6</c:v>
+                  <c:v>5.2700000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9999999999999999E-6</c:v>
+                  <c:v>5.4799999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0000000000000001E-6</c:v>
+                  <c:v>5.5000000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0000000000000001E-6</c:v>
+                  <c:v>5.2899999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.9999999999999998E-6</c:v>
+                  <c:v>5.7399999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.9999999999999998E-6</c:v>
+                  <c:v>5.53E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9999999999999999E-6</c:v>
+                  <c:v>5.2400000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9999999999999999E-6</c:v>
+                  <c:v>5.5500000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.9999999999999998E-6</c:v>
+                  <c:v>6.02E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.0000000000000004E-6</c:v>
+                  <c:v>6.0999999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9999999999999998E-6</c:v>
+                  <c:v>5.7399999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.0000000000000002E-6</c:v>
+                  <c:v>5.3300000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.0000000000000004E-6</c:v>
+                  <c:v>5.8799999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.9999999999999999E-6</c:v>
+                  <c:v>5.4799999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.9999999999999999E-6</c:v>
+                  <c:v>6.29E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.9999999999999999E-6</c:v>
+                  <c:v>6.1700000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.9999999999999999E-6</c:v>
+                  <c:v>5.5999999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.9999999999999996E-6</c:v>
+                  <c:v>5.8E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.0000000000000001E-6</c:v>
+                  <c:v>6.4899999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.0000000000000001E-6</c:v>
+                  <c:v>5.6400000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6.9999999999999999E-6</c:v>
+                  <c:v>5.8699999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.9999999999999998E-6</c:v>
+                  <c:v>6.1899999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.0000000000000004E-6</c:v>
+                  <c:v>5.3600000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.0000000000000004E-6</c:v>
+                  <c:v>5.6800000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.0000000000000004E-6</c:v>
+                  <c:v>6.1899999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.0000000000000002E-6</c:v>
+                  <c:v>5.6499999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.9999999999999999E-6</c:v>
+                  <c:v>5.7499999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.9999999999999996E-6</c:v>
+                  <c:v>5.6599999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>9.0000000000000002E-6</c:v>
+                  <c:v>5.4799999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.0000000000000001E-5</c:v>
+                  <c:v>6.11E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.1E-5</c:v>
+                  <c:v>6.1899999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.2999999999999999E-5</c:v>
+                  <c:v>5.4299999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.5E-5</c:v>
+                  <c:v>5.8799999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.0000000000000002E-5</c:v>
+                  <c:v>6.8900000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.4000000000000001E-5</c:v>
+                  <c:v>5.4600000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.4E-5</c:v>
+                  <c:v>5.7799999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.6999999999999999E-5</c:v>
+                  <c:v>5.9599999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.1999999999999999E-5</c:v>
+                  <c:v>5.7200000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.3000000000000002E-5</c:v>
+                  <c:v>5.5599999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.3000000000000002E-5</c:v>
+                  <c:v>5.9000000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.8000000000000001E-5</c:v>
+                  <c:v>5.3799999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.8999999999999998E-5</c:v>
+                  <c:v>5.4600000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6.4999999999999994E-5</c:v>
+                  <c:v>6.0300000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>8.7999999999999998E-5</c:v>
+                  <c:v>6.3699999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>8.1000000000000004E-5</c:v>
+                  <c:v>5.8100000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.16E-4</c:v>
+                  <c:v>6.3100000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.13E-4</c:v>
+                  <c:v>5.6300000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.26E-4</c:v>
+                  <c:v>6.0300000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.73E-4</c:v>
+                  <c:v>7.6900000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.76E-4</c:v>
+                  <c:v>6.3299999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.1100000000000001E-4</c:v>
+                  <c:v>6.1700000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.2599999999999999E-4</c:v>
+                  <c:v>6.3100000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.8499999999999999E-4</c:v>
+                  <c:v>6.1700000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3.68E-4</c:v>
+                  <c:v>6.3500000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3.5799999999999997E-4</c:v>
+                  <c:v>6.4800000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4.15E-4</c:v>
+                  <c:v>6.2699999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4.9299999999999995E-4</c:v>
+                  <c:v>6.4899999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>5.3700000000000004E-4</c:v>
+                  <c:v>6.78E-4</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>7.1599999999999995E-4</c:v>
+                  <c:v>6.9099999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>7.0500000000000001E-4</c:v>
+                  <c:v>6.9300000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>8.4999999999999995E-4</c:v>
+                  <c:v>7.6499999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>9.3300000000000002E-4</c:v>
+                  <c:v>7.7300000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.1429999999999999E-3</c:v>
+                  <c:v>7.8100000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.408E-3</c:v>
+                  <c:v>8.1400000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.4450000000000001E-3</c:v>
+                  <c:v>8.6700000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.621E-3</c:v>
+                  <c:v>8.9300000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.9629999999999999E-3</c:v>
+                  <c:v>9.7400000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2.6020000000000001E-3</c:v>
+                  <c:v>1.041E-3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2.4520000000000002E-3</c:v>
+                  <c:v>1.155E-3</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>2.8600000000000001E-3</c:v>
+                  <c:v>1.255E-3</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>3.2299999999999998E-3</c:v>
+                  <c:v>1.436E-3</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>3.699E-3</c:v>
+                  <c:v>1.539E-3</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>4.3689999999999996E-3</c:v>
+                  <c:v>1.7520000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>6.4869999999999997E-3</c:v>
+                  <c:v>1.9889999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>6.3359999999999996E-3</c:v>
+                  <c:v>2.2039999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>6.574E-3</c:v>
+                  <c:v>2.7399999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>7.7520000000000002E-3</c:v>
+                  <c:v>2.8210000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>9.1050000000000002E-3</c:v>
+                  <c:v>2.7130000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.307E-2</c:v>
+                  <c:v>3.614E-3</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.5321E-2</c:v>
+                  <c:v>4.104E-3</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.7825000000000001E-2</c:v>
+                  <c:v>4.6940000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>2.0607E-2</c:v>
+                  <c:v>5.2890000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2.4006E-2</c:v>
+                  <c:v>6.1409999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>2.7730000000000001E-2</c:v>
+                  <c:v>7.1910000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>3.2000000000000001E-2</c:v>
+                  <c:v>8.1759999999999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>3.7734999999999998E-2</c:v>
+                  <c:v>9.3950000000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>4.2827999999999998E-2</c:v>
+                  <c:v>1.0668E-2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>4.8481999999999997E-2</c:v>
+                  <c:v>1.2177E-2</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>5.4928999999999999E-2</c:v>
+                  <c:v>1.4237E-2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>6.1462999999999997E-2</c:v>
+                  <c:v>1.6032999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>7.2636999999999993E-2</c:v>
+                  <c:v>2.1826999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>8.3488999999999994E-2</c:v>
+                  <c:v>2.1493999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>9.5599000000000003E-2</c:v>
+                  <c:v>2.4208E-2</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.108642</c:v>
+                  <c:v>2.7564999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.12623300000000001</c:v>
+                  <c:v>3.1628999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.145374</c:v>
+                  <c:v>3.6727000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.17203199999999999</c:v>
+                  <c:v>4.1807999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.19111600000000001</c:v>
+                  <c:v>4.8459000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.21957499999999999</c:v>
+                  <c:v>5.4550000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.25300099999999998</c:v>
+                  <c:v>6.2994999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.290024</c:v>
+                  <c:v>7.2902999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.33310699999999999</c:v>
+                  <c:v>8.3049999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0.38113599999999997</c:v>
+                  <c:v>9.5651E-2</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>0.43836700000000001</c:v>
+                  <c:v>0.10893600000000001</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.50213099999999999</c:v>
+                  <c:v>0.125083</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>0.58169400000000004</c:v>
+                  <c:v>0.14440600000000001</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>0.68053300000000005</c:v>
+                  <c:v>0.16637299999999999</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>0.76647399999999999</c:v>
+                  <c:v>0.19142400000000001</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>0.88116300000000003</c:v>
+                  <c:v>0.219751</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1.009571</c:v>
+                  <c:v>0.251531</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1.170804</c:v>
+                  <c:v>0.28958099999999998</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1.36145</c:v>
+                  <c:v>0.33216000000000001</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1.537642</c:v>
+                  <c:v>0.38455299999999998</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>1.760103</c:v>
+                  <c:v>0.44852900000000001</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>2.0234770000000002</c:v>
+                  <c:v>0.50617599999999996</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>2.3315700000000001</c:v>
+                  <c:v>0.58214900000000003</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>2.6894909999999999</c:v>
+                  <c:v>0.67033200000000004</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>3.0847630000000001</c:v>
+                  <c:v>0.77732599999999996</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>3.5440689999999999</c:v>
+                  <c:v>0.883718</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6018,11 +6019,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93786048"/>
-        <c:axId val="93786624"/>
+        <c:axId val="103962240"/>
+        <c:axId val="103959360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93786048"/>
+        <c:axId val="103962240"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6054,12 +6055,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93786624"/>
+        <c:crossAx val="103959360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93786624"/>
+        <c:axId val="103959360"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6090,7 +6091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93786048"/>
+        <c:crossAx val="103962240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6120,7 +6121,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -6449,8 +6450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J882"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9935,1696 +9936,1696 @@
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="2">
+      <c r="A255" s="4">
         <v>2</v>
       </c>
-      <c r="B255" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="C255" s="2">
+      <c r="B255" s="4">
+        <v>5.7799999999999995E-4</v>
+      </c>
+      <c r="C255" s="4">
+        <v>2.4000000000000001E-5</v>
+      </c>
+      <c r="D255" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="4">
+        <v>3</v>
+      </c>
+      <c r="B256" s="4">
+        <v>5.5999999999999995E-4</v>
+      </c>
+      <c r="C256" s="4">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="D256" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="4">
+        <v>4</v>
+      </c>
+      <c r="B257" s="4">
+        <v>5.2700000000000002E-4</v>
+      </c>
+      <c r="C257" s="4">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D257" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" s="4">
+        <v>5</v>
+      </c>
+      <c r="B258" s="4">
+        <v>5.4799999999999998E-4</v>
+      </c>
+      <c r="C258" s="4">
+        <v>3.3000000000000003E-5</v>
+      </c>
+      <c r="D258" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="4">
+        <v>6</v>
+      </c>
+      <c r="B259" s="4">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="C259" s="4">
+        <v>1.4E-5</v>
+      </c>
+      <c r="D259" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="4">
+        <v>8</v>
+      </c>
+      <c r="B260" s="4">
+        <v>5.2899999999999996E-4</v>
+      </c>
+      <c r="C260" s="4">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D255" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="2">
-        <v>3</v>
-      </c>
-      <c r="B256" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="C256" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D256" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A257" s="2">
-        <v>4</v>
-      </c>
-      <c r="B257" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="C257" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D257" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A258" s="2">
-        <v>5</v>
-      </c>
-      <c r="B258" s="2">
+      <c r="D260" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="4">
+        <v>9</v>
+      </c>
+      <c r="B261" s="4">
+        <v>5.7399999999999997E-4</v>
+      </c>
+      <c r="C261" s="4">
+        <v>6.6000000000000005E-5</v>
+      </c>
+      <c r="D261" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="4">
+        <v>10</v>
+      </c>
+      <c r="B262" s="4">
+        <v>5.53E-4</v>
+      </c>
+      <c r="C262" s="4">
+        <v>1.2E-5</v>
+      </c>
+      <c r="D262" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="4">
+        <v>12</v>
+      </c>
+      <c r="B263" s="4">
+        <v>5.2400000000000005E-4</v>
+      </c>
+      <c r="C263" s="4">
+        <v>3.1999999999999999E-5</v>
+      </c>
+      <c r="D263" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" s="4">
+        <v>13</v>
+      </c>
+      <c r="B264" s="4">
+        <v>5.5500000000000005E-4</v>
+      </c>
+      <c r="C264" s="4">
+        <v>2.3E-5</v>
+      </c>
+      <c r="D264" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" s="4">
+        <v>16</v>
+      </c>
+      <c r="B265" s="4">
+        <v>6.02E-4</v>
+      </c>
+      <c r="C265" s="4">
+        <v>3.1000000000000001E-5</v>
+      </c>
+      <c r="D265" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" s="4">
+        <v>18</v>
+      </c>
+      <c r="B266" s="4">
+        <v>6.0999999999999997E-4</v>
+      </c>
+      <c r="C266" s="4">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="D266" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" s="4">
+        <v>21</v>
+      </c>
+      <c r="B267" s="4">
+        <v>5.7399999999999997E-4</v>
+      </c>
+      <c r="C267" s="4">
+        <v>4.3000000000000002E-5</v>
+      </c>
+      <c r="D267" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" s="4">
+        <v>24</v>
+      </c>
+      <c r="B268" s="4">
+        <v>5.3300000000000005E-4</v>
+      </c>
+      <c r="C268" s="4">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="D268" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" s="4">
+        <v>27</v>
+      </c>
+      <c r="B269" s="4">
+        <v>5.8799999999999998E-4</v>
+      </c>
+      <c r="C269" s="4">
+        <v>4.3999999999999999E-5</v>
+      </c>
+      <c r="D269" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" s="4">
+        <v>32</v>
+      </c>
+      <c r="B270" s="4">
+        <v>5.4799999999999998E-4</v>
+      </c>
+      <c r="C270" s="4">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="D270" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" s="4">
+        <v>36</v>
+      </c>
+      <c r="B271" s="4">
+        <v>6.29E-4</v>
+      </c>
+      <c r="C271" s="4">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="D271" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="4">
+        <v>42</v>
+      </c>
+      <c r="B272" s="4">
+        <v>6.1700000000000004E-4</v>
+      </c>
+      <c r="C272" s="4">
+        <v>1.9000000000000001E-5</v>
+      </c>
+      <c r="D272" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="4">
+        <v>48</v>
+      </c>
+      <c r="B273" s="4">
+        <v>5.5999999999999995E-4</v>
+      </c>
+      <c r="C273" s="4">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="D273" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="4">
+        <v>55</v>
+      </c>
+      <c r="B274" s="4">
+        <v>5.8E-4</v>
+      </c>
+      <c r="C274" s="4">
+        <v>5.7000000000000003E-5</v>
+      </c>
+      <c r="D274" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="4">
+        <v>64</v>
+      </c>
+      <c r="B275" s="4">
+        <v>6.4899999999999995E-4</v>
+      </c>
+      <c r="C275" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="D275" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="4">
+        <v>73</v>
+      </c>
+      <c r="B276" s="4">
+        <v>5.6400000000000005E-4</v>
+      </c>
+      <c r="C276" s="4">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="D276" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" s="4">
+        <v>84</v>
+      </c>
+      <c r="B277" s="4">
+        <v>5.8699999999999996E-4</v>
+      </c>
+      <c r="C277" s="4">
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="D277" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="4">
+        <v>97</v>
+      </c>
+      <c r="B278" s="4">
+        <v>6.1899999999999998E-4</v>
+      </c>
+      <c r="C278" s="4">
+        <v>1.7E-5</v>
+      </c>
+      <c r="D278" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="4">
+        <v>111</v>
+      </c>
+      <c r="B279" s="4">
+        <v>5.3600000000000002E-4</v>
+      </c>
+      <c r="C279" s="4">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="D279" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="4">
+        <v>128</v>
+      </c>
+      <c r="B280" s="4">
+        <v>5.6800000000000004E-4</v>
+      </c>
+      <c r="C280" s="4">
+        <v>4.1E-5</v>
+      </c>
+      <c r="D280" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" s="4">
+        <v>147</v>
+      </c>
+      <c r="B281" s="4">
+        <v>6.1899999999999998E-4</v>
+      </c>
+      <c r="C281" s="4">
+        <v>1.1E-5</v>
+      </c>
+      <c r="D281" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" s="4">
+        <v>168</v>
+      </c>
+      <c r="B282" s="4">
+        <v>5.6499999999999996E-4</v>
+      </c>
+      <c r="C282" s="4">
+        <v>2.6999999999999999E-5</v>
+      </c>
+      <c r="D282" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" s="4">
+        <v>194</v>
+      </c>
+      <c r="B283" s="4">
+        <v>5.7499999999999999E-4</v>
+      </c>
+      <c r="C283" s="4">
+        <v>4.3000000000000002E-5</v>
+      </c>
+      <c r="D283" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" s="4">
+        <v>222</v>
+      </c>
+      <c r="B284" s="4">
+        <v>5.6599999999999999E-4</v>
+      </c>
+      <c r="C284" s="4">
+        <v>3.1000000000000001E-5</v>
+      </c>
+      <c r="D284" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" s="4">
+        <v>256</v>
+      </c>
+      <c r="B285" s="4">
+        <v>5.4799999999999998E-4</v>
+      </c>
+      <c r="C285" s="4">
+        <v>1.2E-5</v>
+      </c>
+      <c r="D285" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" s="4">
+        <v>294</v>
+      </c>
+      <c r="B286" s="4">
+        <v>6.11E-4</v>
+      </c>
+      <c r="C286" s="4">
+        <v>4.1E-5</v>
+      </c>
+      <c r="D286" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" s="4">
+        <v>337</v>
+      </c>
+      <c r="B287" s="4">
+        <v>6.1899999999999998E-4</v>
+      </c>
+      <c r="C287" s="4">
+        <v>7.6000000000000004E-5</v>
+      </c>
+      <c r="D287" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" s="4">
+        <v>388</v>
+      </c>
+      <c r="B288" s="4">
+        <v>5.4299999999999997E-4</v>
+      </c>
+      <c r="C288" s="4">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="D288" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" s="4">
+        <v>445</v>
+      </c>
+      <c r="B289" s="4">
+        <v>5.8799999999999998E-4</v>
+      </c>
+      <c r="C289" s="4">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="D289" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="4">
+        <v>512</v>
+      </c>
+      <c r="B290" s="4">
+        <v>6.8900000000000005E-4</v>
+      </c>
+      <c r="C290" s="4">
+        <v>1.5E-5</v>
+      </c>
+      <c r="D290" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="4">
+        <v>588</v>
+      </c>
+      <c r="B291" s="4">
+        <v>5.4600000000000004E-4</v>
+      </c>
+      <c r="C291" s="4">
+        <v>1.1E-5</v>
+      </c>
+      <c r="D291" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="4">
+        <v>675</v>
+      </c>
+      <c r="B292" s="4">
+        <v>5.7799999999999995E-4</v>
+      </c>
+      <c r="C292" s="4">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="D292" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="4">
+        <v>776</v>
+      </c>
+      <c r="B293" s="4">
+        <v>5.9599999999999996E-4</v>
+      </c>
+      <c r="C293" s="4">
+        <v>3.4E-5</v>
+      </c>
+      <c r="D293" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" s="4">
+        <v>891</v>
+      </c>
+      <c r="B294" s="4">
+        <v>5.7200000000000003E-4</v>
+      </c>
+      <c r="C294" s="4">
+        <v>4.3999999999999999E-5</v>
+      </c>
+      <c r="D294" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" s="4">
+        <v>1024</v>
+      </c>
+      <c r="B295" s="4">
+        <v>5.5599999999999996E-4</v>
+      </c>
+      <c r="C295" s="4">
+        <v>1.8E-5</v>
+      </c>
+      <c r="D295" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="4">
+        <v>1176</v>
+      </c>
+      <c r="B296" s="4">
+        <v>5.9000000000000003E-4</v>
+      </c>
+      <c r="C296" s="4">
+        <v>3.8000000000000002E-5</v>
+      </c>
+      <c r="D296" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" s="4">
+        <v>1351</v>
+      </c>
+      <c r="B297" s="4">
+        <v>5.3799999999999996E-4</v>
+      </c>
+      <c r="C297" s="4">
+        <v>1.5E-5</v>
+      </c>
+      <c r="D297" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="4">
+        <v>1552</v>
+      </c>
+      <c r="B298" s="4">
+        <v>5.4600000000000004E-4</v>
+      </c>
+      <c r="C298" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D298" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="4">
+        <v>1782</v>
+      </c>
+      <c r="B299" s="4">
+        <v>6.0300000000000002E-4</v>
+      </c>
+      <c r="C299" s="4">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="D299" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="4">
+        <v>2048</v>
+      </c>
+      <c r="B300" s="4">
+        <v>6.3699999999999998E-4</v>
+      </c>
+      <c r="C300" s="4">
+        <v>8.7999999999999998E-5</v>
+      </c>
+      <c r="D300" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="4">
+        <v>2352</v>
+      </c>
+      <c r="B301" s="4">
+        <v>5.8100000000000003E-4</v>
+      </c>
+      <c r="C301" s="4">
+        <v>1.8E-5</v>
+      </c>
+      <c r="D301" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="4">
+        <v>2702</v>
+      </c>
+      <c r="B302" s="4">
+        <v>6.3100000000000005E-4</v>
+      </c>
+      <c r="C302" s="4">
+        <v>5.5999999999999999E-5</v>
+      </c>
+      <c r="D302" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="4">
+        <v>3104</v>
+      </c>
+      <c r="B303" s="4">
+        <v>5.6300000000000002E-4</v>
+      </c>
+      <c r="C303" s="4">
+        <v>2.6999999999999999E-5</v>
+      </c>
+      <c r="D303" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" s="4">
+        <v>3565</v>
+      </c>
+      <c r="B304" s="4">
+        <v>6.0300000000000002E-4</v>
+      </c>
+      <c r="C304" s="4">
+        <v>6.2000000000000003E-5</v>
+      </c>
+      <c r="D304" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305" s="4">
+        <v>4096</v>
+      </c>
+      <c r="B305" s="4">
+        <v>7.6900000000000004E-4</v>
+      </c>
+      <c r="C305" s="4">
+        <v>8.7000000000000001E-5</v>
+      </c>
+      <c r="D305" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" s="4">
+        <v>4705</v>
+      </c>
+      <c r="B306" s="4">
+        <v>6.3299999999999999E-4</v>
+      </c>
+      <c r="C306" s="4">
+        <v>2.5999999999999998E-5</v>
+      </c>
+      <c r="D306" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" s="4">
+        <v>5404</v>
+      </c>
+      <c r="B307" s="4">
+        <v>6.1700000000000004E-4</v>
+      </c>
+      <c r="C307" s="4">
+        <v>2.3E-5</v>
+      </c>
+      <c r="D307" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" s="4">
+        <v>6208</v>
+      </c>
+      <c r="B308" s="4">
+        <v>6.3100000000000005E-4</v>
+      </c>
+      <c r="C308" s="4">
+        <v>3.6999999999999998E-5</v>
+      </c>
+      <c r="D308" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" s="4">
+        <v>7131</v>
+      </c>
+      <c r="B309" s="4">
+        <v>6.1700000000000004E-4</v>
+      </c>
+      <c r="C309" s="4">
+        <v>3.1000000000000001E-5</v>
+      </c>
+      <c r="D309" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" s="4">
+        <v>8192</v>
+      </c>
+      <c r="B310" s="4">
+        <v>6.3500000000000004E-4</v>
+      </c>
+      <c r="C310" s="4">
+        <v>3.4E-5</v>
+      </c>
+      <c r="D310" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" s="4">
+        <v>9410</v>
+      </c>
+      <c r="B311" s="4">
+        <v>6.4800000000000003E-4</v>
+      </c>
+      <c r="C311" s="4">
+        <v>2.9E-5</v>
+      </c>
+      <c r="D311" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312" s="4">
+        <v>10809</v>
+      </c>
+      <c r="B312" s="4">
+        <v>6.2699999999999995E-4</v>
+      </c>
+      <c r="C312" s="4">
+        <v>6.9999999999999999E-6</v>
+      </c>
+      <c r="D312" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313" s="4">
+        <v>12416</v>
+      </c>
+      <c r="B313" s="4">
+        <v>6.4899999999999995E-4</v>
+      </c>
+      <c r="C313" s="4">
+        <v>2.4000000000000001E-5</v>
+      </c>
+      <c r="D313" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314" s="4">
+        <v>14263</v>
+      </c>
+      <c r="B314" s="4">
+        <v>6.78E-4</v>
+      </c>
+      <c r="C314" s="4">
+        <v>3.3000000000000003E-5</v>
+      </c>
+      <c r="D314" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315" s="4">
+        <v>16384</v>
+      </c>
+      <c r="B315" s="4">
+        <v>6.9099999999999999E-4</v>
+      </c>
+      <c r="C315" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="D315" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316" s="4">
+        <v>18820</v>
+      </c>
+      <c r="B316" s="4">
+        <v>6.9300000000000004E-4</v>
+      </c>
+      <c r="C316" s="4">
+        <v>1.1E-5</v>
+      </c>
+      <c r="D316" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A317" s="4">
+        <v>21618</v>
+      </c>
+      <c r="B317" s="4">
+        <v>7.6499999999999995E-4</v>
+      </c>
+      <c r="C317" s="4">
+        <v>4.1E-5</v>
+      </c>
+      <c r="D317" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A318" s="4">
+        <v>24833</v>
+      </c>
+      <c r="B318" s="4">
+        <v>7.7300000000000003E-4</v>
+      </c>
+      <c r="C318" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D318" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A319" s="4">
+        <v>28526</v>
+      </c>
+      <c r="B319" s="4">
+        <v>7.8100000000000001E-4</v>
+      </c>
+      <c r="C319" s="4">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="D319" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A320" s="4">
+        <v>32768</v>
+      </c>
+      <c r="B320" s="4">
+        <v>8.1400000000000005E-4</v>
+      </c>
+      <c r="C320" s="4">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="C258" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D258" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A259" s="2">
-        <v>6</v>
-      </c>
-      <c r="B259" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="C259" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D259" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A260" s="2">
-        <v>8</v>
-      </c>
-      <c r="B260" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="C260" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D260" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A261" s="2">
-        <v>9</v>
-      </c>
-      <c r="B261" s="2">
+      <c r="D320" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" s="4">
+        <v>37640</v>
+      </c>
+      <c r="B321" s="4">
+        <v>8.6700000000000004E-4</v>
+      </c>
+      <c r="C321" s="4">
+        <v>1.2E-5</v>
+      </c>
+      <c r="D321" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322" s="4">
+        <v>43237</v>
+      </c>
+      <c r="B322" s="4">
+        <v>8.9300000000000002E-4</v>
+      </c>
+      <c r="C322" s="4">
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="D322" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323" s="4">
+        <v>49667</v>
+      </c>
+      <c r="B323" s="4">
+        <v>9.7400000000000004E-4</v>
+      </c>
+      <c r="C323" s="4">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="C261" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D261" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A262" s="2">
-        <v>10</v>
-      </c>
-      <c r="B262" s="2">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="C262" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D262" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A263" s="2">
-        <v>12</v>
-      </c>
-      <c r="B263" s="2">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="C263" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D263" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A264" s="2">
-        <v>13</v>
-      </c>
-      <c r="B264" s="2">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="C264" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D264" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" s="2">
-        <v>16</v>
-      </c>
-      <c r="B265" s="2">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="C265" s="2">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="D265" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A266" s="2">
-        <v>18</v>
-      </c>
-      <c r="B266" s="2">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="C266" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D266" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" s="2">
-        <v>21</v>
-      </c>
-      <c r="B267" s="2">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="C267" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D267" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A268" s="2">
-        <v>24</v>
-      </c>
-      <c r="B268" s="2">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="C268" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D268" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A269" s="2">
-        <v>27</v>
-      </c>
-      <c r="B269" s="2">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="C269" s="2">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="D269" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A270" s="2">
-        <v>32</v>
-      </c>
-      <c r="B270" s="2">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="C270" s="2">
-        <v>0</v>
-      </c>
-      <c r="D270" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" s="2">
-        <v>36</v>
-      </c>
-      <c r="B271" s="2">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="C271" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D271" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A272" s="2">
-        <v>42</v>
-      </c>
-      <c r="B272" s="2">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="C272" s="2">
-        <v>0</v>
-      </c>
-      <c r="D272" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A273" s="2">
-        <v>48</v>
-      </c>
-      <c r="B273" s="2">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="C273" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D273" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A274" s="2">
-        <v>55</v>
-      </c>
-      <c r="B274" s="2">
-        <v>7.9999999999999996E-6</v>
-      </c>
-      <c r="C274" s="2">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="D274" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A275" s="2">
-        <v>64</v>
-      </c>
-      <c r="B275" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="C275" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D275" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A276" s="2">
-        <v>73</v>
-      </c>
-      <c r="B276" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="C276" s="2">
-        <v>0</v>
-      </c>
-      <c r="D276" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A277" s="2">
-        <v>84</v>
-      </c>
-      <c r="B277" s="2">
-        <v>6.9999999999999999E-6</v>
-      </c>
-      <c r="C277" s="2">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="D277" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A278" s="2">
-        <v>97</v>
-      </c>
-      <c r="B278" s="2">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="C278" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D278" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A279" s="2">
-        <v>111</v>
-      </c>
-      <c r="B279" s="2">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="C279" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D279" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A280" s="2">
-        <v>128</v>
-      </c>
-      <c r="B280" s="2">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="C280" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D280" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A281" s="2">
-        <v>147</v>
-      </c>
-      <c r="B281" s="2">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="C281" s="2">
-        <v>0</v>
-      </c>
-      <c r="D281" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A282" s="2">
-        <v>168</v>
-      </c>
-      <c r="B282" s="2">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="C282" s="2">
-        <v>0</v>
-      </c>
-      <c r="D282" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A283" s="2">
-        <v>194</v>
-      </c>
-      <c r="B283" s="2">
-        <v>6.9999999999999999E-6</v>
-      </c>
-      <c r="C283" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D283" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A284" s="2">
-        <v>222</v>
-      </c>
-      <c r="B284" s="2">
-        <v>7.9999999999999996E-6</v>
-      </c>
-      <c r="C284" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D284" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A285" s="2">
-        <v>256</v>
-      </c>
-      <c r="B285" s="2">
-        <v>9.0000000000000002E-6</v>
-      </c>
-      <c r="C285" s="2">
-        <v>0</v>
-      </c>
-      <c r="D285" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A286" s="2">
-        <v>294</v>
-      </c>
-      <c r="B286" s="2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="C286" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D286" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A287" s="2">
-        <v>337</v>
-      </c>
-      <c r="B287" s="2">
-        <v>1.1E-5</v>
-      </c>
-      <c r="C287" s="2">
-        <v>0</v>
-      </c>
-      <c r="D287" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A288" s="2">
-        <v>388</v>
-      </c>
-      <c r="B288" s="2">
-        <v>1.2999999999999999E-5</v>
-      </c>
-      <c r="C288" s="2">
-        <v>0</v>
-      </c>
-      <c r="D288" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A289" s="2">
-        <v>445</v>
-      </c>
-      <c r="B289" s="2">
-        <v>1.5E-5</v>
-      </c>
-      <c r="C289" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D289" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A290" s="2">
-        <v>512</v>
-      </c>
-      <c r="B290" s="2">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="C290" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="D290" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A291" s="2">
-        <v>588</v>
-      </c>
-      <c r="B291" s="2">
-        <v>2.4000000000000001E-5</v>
-      </c>
-      <c r="C291" s="2">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="D291" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A292" s="2">
-        <v>675</v>
-      </c>
-      <c r="B292" s="2">
-        <v>3.4E-5</v>
-      </c>
-      <c r="C292" s="2">
-        <v>9.0000000000000002E-6</v>
-      </c>
-      <c r="D292" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A293" s="2">
-        <v>776</v>
-      </c>
-      <c r="B293" s="2">
-        <v>2.6999999999999999E-5</v>
-      </c>
-      <c r="C293" s="2">
-        <v>0</v>
-      </c>
-      <c r="D293" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A294" s="2">
-        <v>891</v>
-      </c>
-      <c r="B294" s="2">
+      <c r="D323" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324" s="4">
+        <v>57052</v>
+      </c>
+      <c r="B324" s="4">
+        <v>1.041E-3</v>
+      </c>
+      <c r="C324" s="4">
         <v>3.1999999999999999E-5</v>
       </c>
-      <c r="C294" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="D294" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A295" s="2">
-        <v>1024</v>
-      </c>
-      <c r="B295" s="2">
-        <v>4.3000000000000002E-5</v>
-      </c>
-      <c r="C295" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D295" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A296" s="2">
-        <v>1176</v>
-      </c>
-      <c r="B296" s="2">
-        <v>4.3000000000000002E-5</v>
-      </c>
-      <c r="C296" s="2">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="D296" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A297" s="2">
-        <v>1351</v>
-      </c>
-      <c r="B297" s="2">
+      <c r="D324" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325" s="4">
+        <v>65536</v>
+      </c>
+      <c r="B325" s="4">
+        <v>1.155E-3</v>
+      </c>
+      <c r="C325" s="4">
+        <v>7.6000000000000004E-5</v>
+      </c>
+      <c r="D325" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" s="4">
+        <v>75281</v>
+      </c>
+      <c r="B326" s="4">
+        <v>1.255E-3</v>
+      </c>
+      <c r="C326" s="4">
+        <v>4.6999999999999997E-5</v>
+      </c>
+      <c r="D326" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" s="4">
+        <v>86475</v>
+      </c>
+      <c r="B327" s="4">
+        <v>1.436E-3</v>
+      </c>
+      <c r="C327" s="4">
+        <v>5.5000000000000002E-5</v>
+      </c>
+      <c r="D327" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328" s="4">
+        <v>99334</v>
+      </c>
+      <c r="B328" s="4">
+        <v>1.539E-3</v>
+      </c>
+      <c r="C328" s="4">
+        <v>1.3799999999999999E-4</v>
+      </c>
+      <c r="D328" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329" s="4">
+        <v>114104</v>
+      </c>
+      <c r="B329" s="4">
+        <v>1.7520000000000001E-3</v>
+      </c>
+      <c r="C329" s="4">
+        <v>9.2999999999999997E-5</v>
+      </c>
+      <c r="D329" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330" s="4">
+        <v>131072</v>
+      </c>
+      <c r="B330" s="4">
+        <v>1.9889999999999999E-3</v>
+      </c>
+      <c r="C330" s="4">
+        <v>8.1000000000000004E-5</v>
+      </c>
+      <c r="D330" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="4">
+        <v>150562</v>
+      </c>
+      <c r="B331" s="4">
+        <v>2.2039999999999998E-3</v>
+      </c>
+      <c r="C331" s="4">
+        <v>7.7999999999999999E-5</v>
+      </c>
+      <c r="D331" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" s="4">
+        <v>172950</v>
+      </c>
+      <c r="B332" s="4">
+        <v>2.7399999999999998E-3</v>
+      </c>
+      <c r="C332" s="4">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="D332" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" s="4">
+        <v>198668</v>
+      </c>
+      <c r="B333" s="4">
+        <v>2.8210000000000002E-3</v>
+      </c>
+      <c r="C333" s="4">
+        <v>7.2999999999999999E-5</v>
+      </c>
+      <c r="D333" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334" s="4">
+        <v>228209</v>
+      </c>
+      <c r="B334" s="4">
+        <v>2.7130000000000001E-3</v>
+      </c>
+      <c r="C334" s="4">
+        <v>3.1999999999999999E-5</v>
+      </c>
+      <c r="D334" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335" s="4">
+        <v>262144</v>
+      </c>
+      <c r="B335" s="4">
+        <v>3.614E-3</v>
+      </c>
+      <c r="C335" s="4">
+        <v>1.4E-5</v>
+      </c>
+      <c r="D335" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336" s="4">
+        <v>301124</v>
+      </c>
+      <c r="B336" s="4">
+        <v>4.104E-3</v>
+      </c>
+      <c r="C336" s="4">
+        <v>6.6000000000000005E-5</v>
+      </c>
+      <c r="D336" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" s="4">
+        <v>345901</v>
+      </c>
+      <c r="B337" s="4">
+        <v>4.6940000000000003E-3</v>
+      </c>
+      <c r="C337" s="4">
+        <v>8.7999999999999998E-5</v>
+      </c>
+      <c r="D337" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" s="4">
+        <v>397336</v>
+      </c>
+      <c r="B338" s="4">
+        <v>5.2890000000000003E-3</v>
+      </c>
+      <c r="C338" s="4">
+        <v>1.65E-4</v>
+      </c>
+      <c r="D338" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" s="4">
+        <v>456419</v>
+      </c>
+      <c r="B339" s="4">
+        <v>6.1409999999999998E-3</v>
+      </c>
+      <c r="C339" s="4">
+        <v>8.6000000000000003E-5</v>
+      </c>
+      <c r="D339" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" s="4">
+        <v>524288</v>
+      </c>
+      <c r="B340" s="4">
+        <v>7.1910000000000003E-3</v>
+      </c>
+      <c r="C340" s="4">
+        <v>1.5300000000000001E-4</v>
+      </c>
+      <c r="D340" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" s="4">
+        <v>602248</v>
+      </c>
+      <c r="B341" s="4">
+        <v>8.1759999999999992E-3</v>
+      </c>
+      <c r="C341" s="4">
         <v>4.8000000000000001E-5</v>
       </c>
-      <c r="C297" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D297" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A298" s="2">
-        <v>1552</v>
-      </c>
-      <c r="B298" s="2">
-        <v>5.8999999999999998E-5</v>
-      </c>
-      <c r="C298" s="2">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="D298" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A299" s="2">
-        <v>1782</v>
-      </c>
-      <c r="B299" s="2">
-        <v>6.4999999999999994E-5</v>
-      </c>
-      <c r="C299" s="2">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="D299" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A300" s="2">
-        <v>2048</v>
-      </c>
-      <c r="B300" s="2">
-        <v>8.7999999999999998E-5</v>
-      </c>
-      <c r="C300" s="2">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="D300" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A301" s="2">
-        <v>2352</v>
-      </c>
-      <c r="B301" s="2">
-        <v>8.1000000000000004E-5</v>
-      </c>
-      <c r="C301" s="2">
-        <v>0</v>
-      </c>
-      <c r="D301" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A302" s="2">
-        <v>2702</v>
-      </c>
-      <c r="B302" s="2">
-        <v>1.16E-4</v>
-      </c>
-      <c r="C302" s="2">
-        <v>3.1000000000000001E-5</v>
-      </c>
-      <c r="D302" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A303" s="2">
-        <v>3104</v>
-      </c>
-      <c r="B303" s="2">
-        <v>1.13E-4</v>
-      </c>
-      <c r="C303" s="2">
-        <v>6.9999999999999999E-6</v>
-      </c>
-      <c r="D303" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A304" s="2">
-        <v>3565</v>
-      </c>
-      <c r="B304" s="2">
-        <v>1.26E-4</v>
-      </c>
-      <c r="C304" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="D304" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A305" s="2">
-        <v>4096</v>
-      </c>
-      <c r="B305" s="2">
-        <v>1.73E-4</v>
-      </c>
-      <c r="C305" s="2">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="D305" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A306" s="2">
-        <v>4705</v>
-      </c>
-      <c r="B306" s="2">
-        <v>1.76E-4</v>
-      </c>
-      <c r="C306" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D306" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A307" s="2">
-        <v>5404</v>
-      </c>
-      <c r="B307" s="2">
-        <v>2.1100000000000001E-4</v>
-      </c>
-      <c r="C307" s="2">
-        <v>0</v>
-      </c>
-      <c r="D307" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A308" s="2">
-        <v>6208</v>
-      </c>
-      <c r="B308" s="2">
-        <v>2.2599999999999999E-4</v>
-      </c>
-      <c r="C308" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D308" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A309" s="2">
-        <v>7131</v>
-      </c>
-      <c r="B309" s="2">
-        <v>2.8499999999999999E-4</v>
-      </c>
-      <c r="C309" s="2">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="D309" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A310" s="2">
-        <v>8192</v>
-      </c>
-      <c r="B310" s="2">
-        <v>3.68E-4</v>
-      </c>
-      <c r="C310" s="2">
-        <v>3.6000000000000001E-5</v>
-      </c>
-      <c r="D310" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A311" s="2">
-        <v>9410</v>
-      </c>
-      <c r="B311" s="2">
-        <v>3.5799999999999997E-4</v>
-      </c>
-      <c r="C311" s="2">
-        <v>6.9999999999999999E-6</v>
-      </c>
-      <c r="D311" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A312" s="2">
-        <v>10809</v>
-      </c>
-      <c r="B312" s="2">
-        <v>4.15E-4</v>
-      </c>
-      <c r="C312" s="2">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="D312" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A313" s="2">
-        <v>12416</v>
-      </c>
-      <c r="B313" s="2">
-        <v>4.9299999999999995E-4</v>
-      </c>
-      <c r="C313" s="2">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="D313" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A314" s="2">
-        <v>14263</v>
-      </c>
-      <c r="B314" s="2">
-        <v>5.3700000000000004E-4</v>
-      </c>
-      <c r="C314" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="D314" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A315" s="2">
-        <v>16384</v>
-      </c>
-      <c r="B315" s="2">
-        <v>7.1599999999999995E-4</v>
-      </c>
-      <c r="C315" s="2">
-        <v>1.5999999999999999E-5</v>
-      </c>
-      <c r="D315" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A316" s="2">
-        <v>18820</v>
-      </c>
-      <c r="B316" s="2">
-        <v>7.0500000000000001E-4</v>
-      </c>
-      <c r="C316" s="2">
-        <v>1.4E-5</v>
-      </c>
-      <c r="D316" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A317" s="2">
-        <v>21618</v>
-      </c>
-      <c r="B317" s="2">
-        <v>8.4999999999999995E-4</v>
-      </c>
-      <c r="C317" s="2">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="D317" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A318" s="2">
-        <v>24833</v>
-      </c>
-      <c r="B318" s="2">
-        <v>9.3300000000000002E-4</v>
-      </c>
-      <c r="C318" s="2">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="D318" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A319" s="2">
-        <v>28526</v>
-      </c>
-      <c r="B319" s="2">
-        <v>1.1429999999999999E-3</v>
-      </c>
-      <c r="C319" s="2">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="D319" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A320" s="2">
-        <v>32768</v>
-      </c>
-      <c r="B320" s="2">
-        <v>1.408E-3</v>
-      </c>
-      <c r="C320" s="2">
-        <v>1.7E-5</v>
-      </c>
-      <c r="D320" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A321" s="2">
-        <v>37640</v>
-      </c>
-      <c r="B321" s="2">
-        <v>1.4450000000000001E-3</v>
-      </c>
-      <c r="C321" s="2">
-        <v>1.2999999999999999E-5</v>
-      </c>
-      <c r="D321" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A322" s="2">
-        <v>43237</v>
-      </c>
-      <c r="B322" s="2">
-        <v>1.621E-3</v>
-      </c>
-      <c r="C322" s="2">
-        <v>1.5999999999999999E-5</v>
-      </c>
-      <c r="D322" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A323" s="2">
-        <v>49667</v>
-      </c>
-      <c r="B323" s="2">
-        <v>1.9629999999999999E-3</v>
-      </c>
-      <c r="C323" s="2">
+      <c r="D341" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" s="4">
+        <v>691802</v>
+      </c>
+      <c r="B342" s="4">
+        <v>9.3950000000000006E-3</v>
+      </c>
+      <c r="C342" s="4">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="D342" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343" s="4">
+        <v>794672</v>
+      </c>
+      <c r="B343" s="4">
+        <v>1.0668E-2</v>
+      </c>
+      <c r="C343" s="4">
+        <v>2.9E-5</v>
+      </c>
+      <c r="D343" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344" s="4">
+        <v>912838</v>
+      </c>
+      <c r="B344" s="4">
+        <v>1.2177E-2</v>
+      </c>
+      <c r="C344" s="4">
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="D344" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345" s="4">
+        <v>1048576</v>
+      </c>
+      <c r="B345" s="4">
+        <v>1.4237E-2</v>
+      </c>
+      <c r="C345" s="4">
+        <v>3.01E-4</v>
+      </c>
+      <c r="D345" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346" s="4">
+        <v>1204497</v>
+      </c>
+      <c r="B346" s="4">
+        <v>1.6032999999999999E-2</v>
+      </c>
+      <c r="C346" s="4">
         <v>7.6000000000000004E-5</v>
       </c>
-      <c r="D323" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A324" s="2">
-        <v>57052</v>
-      </c>
-      <c r="B324" s="2">
-        <v>2.6020000000000001E-3</v>
-      </c>
-      <c r="C324" s="2">
-        <v>4.66E-4</v>
-      </c>
-      <c r="D324" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A325" s="2">
-        <v>65536</v>
-      </c>
-      <c r="B325" s="2">
-        <v>2.4520000000000002E-3</v>
-      </c>
-      <c r="C325" s="2">
-        <v>2.5999999999999998E-5</v>
-      </c>
-      <c r="D325" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A326" s="2">
-        <v>75281</v>
-      </c>
-      <c r="B326" s="2">
-        <v>2.8600000000000001E-3</v>
-      </c>
-      <c r="C326" s="2">
-        <v>1.2E-5</v>
-      </c>
-      <c r="D326" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A327" s="2">
-        <v>86475</v>
-      </c>
-      <c r="B327" s="2">
-        <v>3.2299999999999998E-3</v>
-      </c>
-      <c r="C327" s="2">
-        <v>9.0000000000000002E-6</v>
-      </c>
-      <c r="D327" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A328" s="2">
-        <v>99334</v>
-      </c>
-      <c r="B328" s="2">
-        <v>3.699E-3</v>
-      </c>
-      <c r="C328" s="2">
-        <v>2.0999999999999999E-5</v>
-      </c>
-      <c r="D328" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A329" s="2">
-        <v>114104</v>
-      </c>
-      <c r="B329" s="2">
-        <v>4.3689999999999996E-3</v>
-      </c>
-      <c r="C329" s="2">
-        <v>6.3999999999999997E-5</v>
-      </c>
-      <c r="D329" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A330" s="2">
-        <v>131072</v>
-      </c>
-      <c r="B330" s="2">
-        <v>6.4869999999999997E-3</v>
-      </c>
-      <c r="C330" s="2">
-        <v>9.7999999999999997E-5</v>
-      </c>
-      <c r="D330" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A331" s="2">
-        <v>150562</v>
-      </c>
-      <c r="B331" s="2">
-        <v>6.3359999999999996E-3</v>
-      </c>
-      <c r="C331" s="2">
-        <v>1.55E-4</v>
-      </c>
-      <c r="D331" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A332" s="2">
-        <v>172950</v>
-      </c>
-      <c r="B332" s="2">
-        <v>6.574E-3</v>
-      </c>
-      <c r="C332" s="2">
-        <v>2.4699999999999999E-4</v>
-      </c>
-      <c r="D332" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A333" s="2">
-        <v>198668</v>
-      </c>
-      <c r="B333" s="2">
-        <v>7.7520000000000002E-3</v>
-      </c>
-      <c r="C333" s="2">
-        <v>2.9E-5</v>
-      </c>
-      <c r="D333" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A334" s="2">
-        <v>228209</v>
-      </c>
-      <c r="B334" s="2">
-        <v>9.1050000000000002E-3</v>
-      </c>
-      <c r="C334" s="2">
-        <v>1.18E-4</v>
-      </c>
-      <c r="D334" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A335" s="2">
-        <v>262144</v>
-      </c>
-      <c r="B335" s="2">
-        <v>1.307E-2</v>
-      </c>
-      <c r="C335" s="2">
-        <v>9.0000000000000006E-5</v>
-      </c>
-      <c r="D335" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A336" s="2">
-        <v>301124</v>
-      </c>
-      <c r="B336" s="2">
-        <v>1.5321E-2</v>
-      </c>
-      <c r="C336" s="2">
-        <v>1.15E-4</v>
-      </c>
-      <c r="D336" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A337" s="2">
-        <v>345901</v>
-      </c>
-      <c r="B337" s="2">
-        <v>1.7825000000000001E-2</v>
-      </c>
-      <c r="C337" s="2">
-        <v>3.4999999999999997E-5</v>
-      </c>
-      <c r="D337" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A338" s="2">
-        <v>397336</v>
-      </c>
-      <c r="B338" s="2">
-        <v>2.0607E-2</v>
-      </c>
-      <c r="C338" s="2">
-        <v>1.47E-4</v>
-      </c>
-      <c r="D338" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A339" s="2">
-        <v>456419</v>
-      </c>
-      <c r="B339" s="2">
-        <v>2.4006E-2</v>
-      </c>
-      <c r="C339" s="2">
-        <v>1.22E-4</v>
-      </c>
-      <c r="D339" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A340" s="2">
-        <v>524288</v>
-      </c>
-      <c r="B340" s="2">
-        <v>2.7730000000000001E-2</v>
-      </c>
-      <c r="C340" s="2">
-        <v>3.6900000000000002E-4</v>
-      </c>
-      <c r="D340" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A341" s="2">
-        <v>602248</v>
-      </c>
-      <c r="B341" s="2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C341" s="2">
-        <v>2.52E-4</v>
-      </c>
-      <c r="D341" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A342" s="2">
-        <v>691802</v>
-      </c>
-      <c r="B342" s="2">
-        <v>3.7734999999999998E-2</v>
-      </c>
-      <c r="C342" s="2">
-        <v>7.5799999999999999E-4</v>
-      </c>
-      <c r="D342" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A343" s="2">
-        <v>794672</v>
-      </c>
-      <c r="B343" s="2">
-        <v>4.2827999999999998E-2</v>
-      </c>
-      <c r="C343" s="2">
-        <v>1.5200000000000001E-4</v>
-      </c>
-      <c r="D343" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A344" s="2">
-        <v>912838</v>
-      </c>
-      <c r="B344" s="2">
-        <v>4.8481999999999997E-2</v>
-      </c>
-      <c r="C344" s="2">
-        <v>4.6700000000000002E-4</v>
-      </c>
-      <c r="D344" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A345" s="2">
-        <v>1048576</v>
-      </c>
-      <c r="B345" s="2">
-        <v>5.4928999999999999E-2</v>
-      </c>
-      <c r="C345" s="2">
-        <v>2.7799999999999998E-4</v>
-      </c>
-      <c r="D345" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A346" s="2">
-        <v>1204497</v>
-      </c>
-      <c r="B346" s="2">
-        <v>6.1462999999999997E-2</v>
-      </c>
-      <c r="C346" s="2">
-        <v>2.3700000000000001E-3</v>
-      </c>
-      <c r="D346" s="2" t="s">
+      <c r="D346" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A347" s="2">
+      <c r="A347" s="4">
         <v>1383604</v>
       </c>
-      <c r="B347" s="2">
-        <v>7.2636999999999993E-2</v>
-      </c>
-      <c r="C347" s="2">
-        <v>3.57E-4</v>
-      </c>
-      <c r="D347" s="2" t="s">
+      <c r="B347" s="4">
+        <v>2.1826999999999999E-2</v>
+      </c>
+      <c r="C347" s="4">
+        <v>4.2929999999999999E-3</v>
+      </c>
+      <c r="D347" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A348" s="2">
+      <c r="A348" s="4">
         <v>1589344</v>
       </c>
-      <c r="B348" s="2">
-        <v>8.3488999999999994E-2</v>
-      </c>
-      <c r="C348" s="2">
-        <v>2.92E-4</v>
-      </c>
-      <c r="D348" s="2" t="s">
+      <c r="B348" s="4">
+        <v>2.1493999999999999E-2</v>
+      </c>
+      <c r="C348" s="4">
+        <v>1.0900000000000001E-4</v>
+      </c>
+      <c r="D348" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A349" s="2">
+      <c r="A349" s="4">
         <v>1825676</v>
       </c>
-      <c r="B349" s="2">
-        <v>9.5599000000000003E-2</v>
-      </c>
-      <c r="C349" s="2">
-        <v>3.6999999999999998E-5</v>
-      </c>
-      <c r="D349" s="2" t="s">
+      <c r="B349" s="4">
+        <v>2.4208E-2</v>
+      </c>
+      <c r="C349" s="4">
+        <v>4.1800000000000002E-4</v>
+      </c>
+      <c r="D349" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A350" s="2">
+      <c r="A350" s="4">
         <v>2097152</v>
       </c>
-      <c r="B350" s="2">
-        <v>0.108642</v>
-      </c>
-      <c r="C350" s="2">
-        <v>2.0609999999999999E-3</v>
-      </c>
-      <c r="D350" s="2" t="s">
+      <c r="B350" s="4">
+        <v>2.7564999999999999E-2</v>
+      </c>
+      <c r="C350" s="4">
+        <v>6.2000000000000003E-5</v>
+      </c>
+      <c r="D350" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A351" s="2">
+      <c r="A351" s="4">
         <v>2408995</v>
       </c>
-      <c r="B351" s="2">
-        <v>0.12623300000000001</v>
-      </c>
-      <c r="C351" s="2">
-        <v>1.6000000000000001E-4</v>
-      </c>
-      <c r="D351" s="2" t="s">
+      <c r="B351" s="4">
+        <v>3.1628999999999997E-2</v>
+      </c>
+      <c r="C351" s="4">
+        <v>2.7500000000000002E-4</v>
+      </c>
+      <c r="D351" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A352" s="2">
+      <c r="A352" s="4">
         <v>2767208</v>
       </c>
-      <c r="B352" s="2">
-        <v>0.145374</v>
-      </c>
-      <c r="C352" s="2">
-        <v>3.4000000000000002E-4</v>
-      </c>
-      <c r="D352" s="2" t="s">
+      <c r="B352" s="4">
+        <v>3.6727000000000003E-2</v>
+      </c>
+      <c r="C352" s="4">
+        <v>2.6899999999999998E-4</v>
+      </c>
+      <c r="D352" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A353" s="2">
+      <c r="A353" s="4">
         <v>3178688</v>
       </c>
-      <c r="B353" s="2">
-        <v>0.17203199999999999</v>
-      </c>
-      <c r="C353" s="2">
-        <v>7.6600000000000001E-3</v>
-      </c>
-      <c r="D353" s="2" t="s">
+      <c r="B353" s="4">
+        <v>4.1807999999999998E-2</v>
+      </c>
+      <c r="C353" s="4">
+        <v>2.43E-4</v>
+      </c>
+      <c r="D353" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A354" s="2">
+      <c r="A354" s="4">
         <v>3651353</v>
       </c>
-      <c r="B354" s="2">
-        <v>0.19111600000000001</v>
-      </c>
-      <c r="C354" s="2">
-        <v>4.9399999999999997E-4</v>
-      </c>
-      <c r="D354" s="2" t="s">
+      <c r="B354" s="4">
+        <v>4.8459000000000002E-2</v>
+      </c>
+      <c r="C354" s="4">
+        <v>1.64E-4</v>
+      </c>
+      <c r="D354" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A355" s="2">
+      <c r="A355" s="4">
         <v>4194304</v>
       </c>
-      <c r="B355" s="2">
-        <v>0.21957499999999999</v>
-      </c>
-      <c r="C355" s="2">
-        <v>3.1100000000000002E-4</v>
-      </c>
-      <c r="D355" s="2" t="s">
+      <c r="B355" s="4">
+        <v>5.4550000000000001E-2</v>
+      </c>
+      <c r="C355" s="4">
+        <v>8.3999999999999995E-5</v>
+      </c>
+      <c r="D355" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A356" s="2">
+      <c r="A356" s="4">
         <v>4817990</v>
       </c>
-      <c r="B356" s="2">
-        <v>0.25300099999999998</v>
-      </c>
-      <c r="C356" s="2">
-        <v>8.4999999999999995E-4</v>
-      </c>
-      <c r="D356" s="2" t="s">
+      <c r="B356" s="4">
+        <v>6.2994999999999995E-2</v>
+      </c>
+      <c r="C356" s="4">
+        <v>4.8500000000000003E-4</v>
+      </c>
+      <c r="D356" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A357" s="2">
+      <c r="A357" s="4">
         <v>5534417</v>
       </c>
-      <c r="B357" s="2">
-        <v>0.290024</v>
-      </c>
-      <c r="C357" s="2">
-        <v>4.37E-4</v>
-      </c>
-      <c r="D357" s="2" t="s">
+      <c r="B357" s="4">
+        <v>7.2902999999999996E-2</v>
+      </c>
+      <c r="C357" s="4">
+        <v>1.057E-3</v>
+      </c>
+      <c r="D357" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A358" s="2">
+      <c r="A358" s="4">
         <v>6357376</v>
       </c>
-      <c r="B358" s="2">
-        <v>0.33310699999999999</v>
-      </c>
-      <c r="C358" s="2">
-        <v>7.67E-4</v>
-      </c>
-      <c r="D358" s="2" t="s">
+      <c r="B358" s="4">
+        <v>8.3049999999999999E-2</v>
+      </c>
+      <c r="C358" s="4">
+        <v>1.1900000000000001E-4</v>
+      </c>
+      <c r="D358" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A359" s="2">
+      <c r="A359" s="4">
         <v>7302707</v>
       </c>
-      <c r="B359" s="2">
-        <v>0.38113599999999997</v>
-      </c>
-      <c r="C359" s="2">
-        <v>6.1879999999999999E-3</v>
-      </c>
-      <c r="D359" s="2" t="s">
+      <c r="B359" s="4">
+        <v>9.5651E-2</v>
+      </c>
+      <c r="C359" s="4">
+        <v>7.6599999999999997E-4</v>
+      </c>
+      <c r="D359" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A360" s="2">
+      <c r="A360" s="4">
         <v>8388608</v>
       </c>
-      <c r="B360" s="2">
-        <v>0.43836700000000001</v>
-      </c>
-      <c r="C360" s="2">
-        <v>1.256E-3</v>
-      </c>
-      <c r="D360" s="2" t="s">
+      <c r="B360" s="4">
+        <v>0.10893600000000001</v>
+      </c>
+      <c r="C360" s="4">
+        <v>2.5099999999999998E-4</v>
+      </c>
+      <c r="D360" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A361" s="2">
+      <c r="A361" s="4">
         <v>9635980</v>
       </c>
-      <c r="B361" s="2">
-        <v>0.50213099999999999</v>
-      </c>
-      <c r="C361" s="2">
-        <v>4.5989999999999998E-3</v>
-      </c>
-      <c r="D361" s="2" t="s">
+      <c r="B361" s="4">
+        <v>0.125083</v>
+      </c>
+      <c r="C361" s="4">
+        <v>7.2999999999999996E-4</v>
+      </c>
+      <c r="D361" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A362" s="2">
+      <c r="A362" s="4">
         <v>11068834</v>
       </c>
-      <c r="B362" s="2">
-        <v>0.58169400000000004</v>
-      </c>
-      <c r="C362" s="2">
-        <v>3.28E-4</v>
-      </c>
-      <c r="D362" s="2" t="s">
+      <c r="B362" s="4">
+        <v>0.14440600000000001</v>
+      </c>
+      <c r="C362" s="4">
+        <v>2.05E-4</v>
+      </c>
+      <c r="D362" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A363" s="2">
+      <c r="A363" s="4">
         <v>12714752</v>
       </c>
-      <c r="B363" s="2">
-        <v>0.68053300000000005</v>
-      </c>
-      <c r="C363" s="2">
-        <v>1.9795E-2</v>
-      </c>
-      <c r="D363" s="2" t="s">
+      <c r="B363" s="4">
+        <v>0.16637299999999999</v>
+      </c>
+      <c r="C363" s="4">
+        <v>1.024E-3</v>
+      </c>
+      <c r="D363" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A364" s="2">
+      <c r="A364" s="4">
         <v>14605414</v>
       </c>
-      <c r="B364" s="2">
-        <v>0.76647399999999999</v>
-      </c>
-      <c r="C364" s="2">
-        <v>1.3129999999999999E-3</v>
-      </c>
-      <c r="D364" s="2" t="s">
+      <c r="B364" s="4">
+        <v>0.19142400000000001</v>
+      </c>
+      <c r="C364" s="4">
+        <v>1.6930000000000001E-3</v>
+      </c>
+      <c r="D364" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A365" s="2">
+      <c r="A365" s="4">
         <v>16777216</v>
       </c>
-      <c r="B365" s="2">
-        <v>0.88116300000000003</v>
-      </c>
-      <c r="C365" s="2">
-        <v>1.5510000000000001E-3</v>
-      </c>
-      <c r="D365" s="2" t="s">
+      <c r="B365" s="4">
+        <v>0.219751</v>
+      </c>
+      <c r="C365" s="4">
+        <v>1.284E-3</v>
+      </c>
+      <c r="D365" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A366" s="2">
+      <c r="A366" s="4">
         <v>19271960</v>
       </c>
-      <c r="B366" s="2">
-        <v>1.009571</v>
-      </c>
-      <c r="C366" s="2">
-        <v>4.836E-3</v>
-      </c>
-      <c r="D366" s="2" t="s">
+      <c r="B366" s="4">
+        <v>0.251531</v>
+      </c>
+      <c r="C366" s="4">
+        <v>4.1100000000000002E-4</v>
+      </c>
+      <c r="D366" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A367" s="2">
+      <c r="A367" s="4">
         <v>22137669</v>
       </c>
-      <c r="B367" s="2">
-        <v>1.170804</v>
-      </c>
-      <c r="C367" s="2">
-        <v>1.3642E-2</v>
-      </c>
-      <c r="D367" s="2" t="s">
+      <c r="B367" s="4">
+        <v>0.28958099999999998</v>
+      </c>
+      <c r="C367" s="4">
+        <v>4.4900000000000002E-4</v>
+      </c>
+      <c r="D367" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A368" s="2">
+      <c r="A368" s="4">
         <v>25429504</v>
       </c>
-      <c r="B368" s="2">
-        <v>1.36145</v>
-      </c>
-      <c r="C368" s="2">
-        <v>3.7118999999999999E-2</v>
-      </c>
-      <c r="D368" s="2" t="s">
+      <c r="B368" s="4">
+        <v>0.33216000000000001</v>
+      </c>
+      <c r="C368" s="4">
+        <v>1.358E-3</v>
+      </c>
+      <c r="D368" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A369" s="2">
+      <c r="A369" s="4">
         <v>29210829</v>
       </c>
-      <c r="B369" s="2">
-        <v>1.537642</v>
-      </c>
-      <c r="C369" s="2">
-        <v>2.8930000000000002E-3</v>
-      </c>
-      <c r="D369" s="2" t="s">
+      <c r="B369" s="4">
+        <v>0.38455299999999998</v>
+      </c>
+      <c r="C369" s="4">
+        <v>2.235E-3</v>
+      </c>
+      <c r="D369" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="370" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A370" s="2">
+      <c r="A370" s="4">
         <v>33554432</v>
       </c>
-      <c r="B370" s="2">
-        <v>1.760103</v>
-      </c>
-      <c r="C370" s="2">
-        <v>2.2251E-2</v>
-      </c>
-      <c r="D370" s="2" t="s">
+      <c r="B370" s="4">
+        <v>0.44852900000000001</v>
+      </c>
+      <c r="C370" s="4">
+        <v>7.3210000000000003E-3</v>
+      </c>
+      <c r="D370" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="371" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A371" s="2">
+      <c r="A371" s="4">
         <v>38543920</v>
       </c>
-      <c r="B371" s="2">
-        <v>2.0234770000000002</v>
-      </c>
-      <c r="C371" s="2">
-        <v>1.0675E-2</v>
-      </c>
-      <c r="D371" s="2" t="s">
+      <c r="B371" s="4">
+        <v>0.50617599999999996</v>
+      </c>
+      <c r="C371" s="4">
+        <v>7.6599999999999997E-4</v>
+      </c>
+      <c r="D371" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="372" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A372" s="2">
+      <c r="A372" s="4">
         <v>44275338</v>
       </c>
-      <c r="B372" s="2">
-        <v>2.3315700000000001</v>
-      </c>
-      <c r="C372" s="2">
-        <v>1.2482999999999999E-2</v>
-      </c>
-      <c r="D372" s="2" t="s">
+      <c r="B372" s="4">
+        <v>0.58214900000000003</v>
+      </c>
+      <c r="C372" s="4">
+        <v>3.7190000000000001E-3</v>
+      </c>
+      <c r="D372" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="373" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A373" s="2">
+      <c r="A373" s="4">
         <v>50859008</v>
       </c>
-      <c r="B373" s="2">
-        <v>2.6894909999999999</v>
-      </c>
-      <c r="C373" s="2">
-        <v>2.0986999999999999E-2</v>
-      </c>
-      <c r="D373" s="2" t="s">
+      <c r="B373" s="4">
+        <v>0.67033200000000004</v>
+      </c>
+      <c r="C373" s="4">
+        <v>6.0759999999999998E-3</v>
+      </c>
+      <c r="D373" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="374" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A374" s="2">
+      <c r="A374" s="4">
         <v>58421659</v>
       </c>
-      <c r="B374" s="2">
-        <v>3.0847630000000001</v>
-      </c>
-      <c r="C374" s="2">
-        <v>4.7828000000000002E-2</v>
-      </c>
-      <c r="D374" s="2" t="s">
+      <c r="B374" s="4">
+        <v>0.77732599999999996</v>
+      </c>
+      <c r="C374" s="4">
+        <v>1.5963000000000001E-2</v>
+      </c>
+      <c r="D374" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="375" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A375" s="2">
+      <c r="A375" s="4">
         <v>67108864</v>
       </c>
-      <c r="B375" s="2">
-        <v>3.5440689999999999</v>
-      </c>
-      <c r="C375" s="2">
-        <v>1.6445000000000001E-2</v>
-      </c>
-      <c r="D375" s="2" t="s">
+      <c r="B375" s="4">
+        <v>0.883718</v>
+      </c>
+      <c r="C375" s="4">
+        <v>3.137E-3</v>
+      </c>
+      <c r="D375" s="4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Added radix sort vector to benchmark data and chart * Finished radix sort chapters
</commit_message>
<xml_diff>
--- a/latex/charts/2013_08_15_sort_high_res.xlsx
+++ b/latex/charts/2013_08_15_sort_high_res.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="24">
   <si>
     <t>Runner built on Jul 21 2013 02:44:35</t>
   </si>
@@ -64,9 +64,6 @@
     <t>cleanup time</t>
   </si>
   <si>
-    <t>Total runtime 27min 57s 162ms</t>
-  </si>
-  <si>
     <t>qsort</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>Radix sort local</t>
+  </si>
+  <si>
+    <t>Radix sort local vector</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2210,6 +2211,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -4499,6 +4505,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -5262,6 +5273,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -6005,6 +6021,774 @@
                 </c:pt>
                 <c:pt idx="120">
                   <c:v>8.4422650000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats!$A$881:$B$881</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Radix sort local vector GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>stats!$A$884:$A$1004</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="121"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>776</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>891</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1176</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1351</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1552</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1782</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2352</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2702</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3104</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3565</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4705</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5404</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6208</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7131</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9410</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>10809</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>12416</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>14263</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>18820</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>21618</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>24833</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>28526</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>37640</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>43237</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>49667</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>57052</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>75281</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>86475</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>99334</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>114104</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>150562</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>172950</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>198668</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>228209</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>301124</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>345901</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>397336</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>456419</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>602248</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>691802</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>794672</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>912838</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1204497</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1383604</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1589344</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1825676</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2408995</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2767208</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3178688</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3651353</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>4817990</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>5534417</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>6357376</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>7302707</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>9635980</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>11068834</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>12714752</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>14605414</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>19271960</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>22137669</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>25429504</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>29210829</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>38543920</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>44275338</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>50859008</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>58421659</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>67108864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>stats!$I$884:$I$1004</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="121"/>
+                <c:pt idx="0">
+                  <c:v>6.3930000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9909999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1219999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5690000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5690000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.1890000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4549999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.744E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.8390000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5290000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.0720000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0369999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.8129999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.731E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.7889999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.6499999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.6299999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5040000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.8700000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.4140000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.5129999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.457E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.1399999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.4279999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.6899999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.4819999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.1219999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.8570000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.6979999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.1469999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.855E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.4339999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.6639999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.6959999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.5269999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.6059999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.0520000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.0639999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.8630000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.4660000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.7699999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.5120000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.7400000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.6340000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.4409999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.8199999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.4349999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.1089999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.2399999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.6579999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.5230000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.0930000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.4070000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.4869999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.3379999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.1749999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.9659999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.6730000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.3860000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.5979999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.1700000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.4840000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.9769999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.4599999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.6889999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.6049999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.1679999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.8719999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.4070000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.1040000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6.1859999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6.7999999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.1510000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.6480000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>8.3330000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.5259999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.8789999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.0444999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.1001E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.089E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.1143E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.4154999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.5313999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.7204000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.8034000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.9841000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.3942999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.6058999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.8244999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.1587999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.5349999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4.1377999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4.6786000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.1434000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>6.0414000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>6.5599000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>7.5936000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>8.591E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.9623000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.112918</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.127582</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.14842900000000001</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.16816800000000001</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.19503200000000001</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.22329399999999999</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.25682100000000002</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.29662899999999998</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.33914299999999997</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.38895099999999999</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.44506000000000001</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.51392400000000005</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.588117</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.67390000000000005</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.77773899999999996</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.89144900000000005</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1.0191159999999999</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1.1738139999999999</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.347224</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.54203</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.7677419999999999</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2.0352649999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6019,11 +6803,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="103962240"/>
-        <c:axId val="103959360"/>
+        <c:axId val="142100736"/>
+        <c:axId val="71572224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103962240"/>
+        <c:axId val="142100736"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6055,12 +6839,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103959360"/>
+        <c:crossAx val="71572224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103959360"/>
+        <c:axId val="71572224"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6091,7 +6875,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103962240"/>
+        <c:crossAx val="142100736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6448,10 +7232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J882"/>
+  <dimension ref="A1:J1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G880" sqref="G880"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6480,7 +7264,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -8196,7 +8980,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B129" t="s">
         <v>2</v>
@@ -9913,7 +10697,7 @@
     <row r="252" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="253" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>2</v>
@@ -11631,10 +12415,10 @@
     </row>
     <row r="377" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
+        <v>18</v>
+      </c>
+      <c r="B377" t="s">
         <v>19</v>
-      </c>
-      <c r="B377" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="378" spans="1:10" x14ac:dyDescent="0.25">
@@ -15559,10 +16343,10 @@
     </row>
     <row r="503" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B503" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="504" spans="1:10" x14ac:dyDescent="0.25">
@@ -19487,10 +20271,10 @@
     </row>
     <row r="629" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A629" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B629" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C629" s="3"/>
       <c r="D629" s="3"/>
@@ -23439,10 +24223,10 @@
     </row>
     <row r="755" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A755" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B755" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C755" s="3"/>
       <c r="D755" s="3"/>
@@ -27389,19 +28173,3949 @@
       <c r="I879" s="3"/>
       <c r="J879" s="3"/>
     </row>
+    <row r="881" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A881" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B881" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C881" s="5"/>
+      <c r="D881" s="5"/>
+      <c r="E881" s="5"/>
+      <c r="F881" s="5"/>
+      <c r="G881" s="5"/>
+      <c r="H881" s="5"/>
+      <c r="I881" s="5"/>
+      <c r="J881" s="5"/>
+    </row>
     <row r="882" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A882" s="3" t="s">
+      <c r="A882" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B882" s="5">
+        <v>0.19917399999999999</v>
+      </c>
+      <c r="C882" s="5"/>
+      <c r="D882" s="5"/>
+      <c r="E882" s="5"/>
+      <c r="F882" s="5"/>
+      <c r="G882" s="5"/>
+      <c r="H882" s="5"/>
+      <c r="I882" s="5"/>
+      <c r="J882" s="5"/>
+    </row>
+    <row r="883" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A883" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B883" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C883" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D883" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E883" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F883" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G883" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H883" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I883" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J883" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="884" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A884" s="5">
+        <v>2</v>
+      </c>
+      <c r="B884" s="5">
+        <v>1.235E-3</v>
+      </c>
+      <c r="C884" s="5">
+        <v>1.1659999999999999E-3</v>
+      </c>
+      <c r="D884" s="5">
+        <v>4.8780000000000004E-3</v>
+      </c>
+      <c r="E884" s="5">
+        <v>2.0709999999999999E-3</v>
+      </c>
+      <c r="F884" s="5">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="G884" s="5">
+        <v>1.45E-4</v>
+      </c>
+      <c r="H884" s="5">
+        <v>256</v>
+      </c>
+      <c r="I884" s="5">
+        <v>6.3930000000000002E-3</v>
+      </c>
+      <c r="J884" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="885" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A885" s="5">
+        <v>3</v>
+      </c>
+      <c r="B885" s="5">
+        <v>3.8400000000000001E-4</v>
+      </c>
+      <c r="C885" s="5">
+        <v>5.7000000000000003E-5</v>
+      </c>
+      <c r="D885" s="5">
+        <v>4.4130000000000003E-3</v>
+      </c>
+      <c r="E885" s="5">
+        <v>1.343E-3</v>
+      </c>
+      <c r="F885" s="5">
+        <v>1.94E-4</v>
+      </c>
+      <c r="G885" s="5">
+        <v>4.1999999999999998E-5</v>
+      </c>
+      <c r="H885" s="5">
+        <v>256</v>
+      </c>
+      <c r="I885" s="5">
+        <v>4.9909999999999998E-3</v>
+      </c>
+      <c r="J885" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="886" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A886" s="5">
+        <v>4</v>
+      </c>
+      <c r="B886" s="5">
+        <v>6.3699999999999998E-4</v>
+      </c>
+      <c r="C886" s="5">
+        <v>1.55E-4</v>
+      </c>
+      <c r="D886" s="5">
+        <v>4.0489999999999996E-3</v>
+      </c>
+      <c r="E886" s="5">
+        <v>4.6700000000000002E-4</v>
+      </c>
+      <c r="F886" s="5">
+        <v>4.35E-4</v>
+      </c>
+      <c r="G886" s="5">
+        <v>6.7999999999999999E-5</v>
+      </c>
+      <c r="H886" s="5">
+        <v>256</v>
+      </c>
+      <c r="I886" s="5">
+        <v>5.1219999999999998E-3</v>
+      </c>
+      <c r="J886" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="887" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A887" s="5">
+        <v>5</v>
+      </c>
+      <c r="B887" s="5">
+        <v>4.73E-4</v>
+      </c>
+      <c r="C887" s="5">
+        <v>1.21E-4</v>
+      </c>
+      <c r="D887" s="5">
+        <v>4.5950000000000001E-3</v>
+      </c>
+      <c r="E887" s="5">
+        <v>1.291E-3</v>
+      </c>
+      <c r="F887" s="5">
+        <v>5.0100000000000003E-4</v>
+      </c>
+      <c r="G887" s="5">
+        <v>1.1E-4</v>
+      </c>
+      <c r="H887" s="5">
+        <v>256</v>
+      </c>
+      <c r="I887" s="5">
+        <v>5.5690000000000002E-3</v>
+      </c>
+      <c r="J887" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="888" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A888" s="5">
+        <v>6</v>
+      </c>
+      <c r="B888" s="5">
+        <v>1.4350000000000001E-3</v>
+      </c>
+      <c r="C888" s="5">
+        <v>8.9400000000000005E-4</v>
+      </c>
+      <c r="D888" s="5">
+        <v>3.676E-3</v>
+      </c>
+      <c r="E888" s="5">
+        <v>7.3999999999999996E-5</v>
+      </c>
+      <c r="F888" s="5">
+        <v>4.5899999999999999E-4</v>
+      </c>
+      <c r="G888" s="5">
+        <v>2.1100000000000001E-4</v>
+      </c>
+      <c r="H888" s="5">
+        <v>256</v>
+      </c>
+      <c r="I888" s="5">
+        <v>5.5690000000000002E-3</v>
+      </c>
+      <c r="J888" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="889" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A889" s="5">
+        <v>8</v>
+      </c>
+      <c r="B889" s="5">
+        <v>1.702E-3</v>
+      </c>
+      <c r="C889" s="5">
+        <v>1.531E-3</v>
+      </c>
+      <c r="D889" s="5">
+        <v>4.0109999999999998E-3</v>
+      </c>
+      <c r="E889" s="5">
+        <v>2.4499999999999999E-4</v>
+      </c>
+      <c r="F889" s="5">
+        <v>4.7600000000000002E-4</v>
+      </c>
+      <c r="G889" s="5">
+        <v>4.3999999999999999E-5</v>
+      </c>
+      <c r="H889" s="5">
+        <v>256</v>
+      </c>
+      <c r="I889" s="5">
+        <v>6.1890000000000001E-3</v>
+      </c>
+      <c r="J889" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="890" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A890" s="5">
+        <v>9</v>
+      </c>
+      <c r="B890" s="5">
+        <v>6.0700000000000001E-4</v>
+      </c>
+      <c r="C890" s="5">
+        <v>1.02E-4</v>
+      </c>
+      <c r="D890" s="5">
+        <v>4.3140000000000001E-3</v>
+      </c>
+      <c r="E890" s="5">
+        <v>8.6700000000000004E-4</v>
+      </c>
+      <c r="F890" s="5">
+        <v>5.3399999999999997E-4</v>
+      </c>
+      <c r="G890" s="5">
+        <v>8.8999999999999995E-5</v>
+      </c>
+      <c r="H890" s="5">
+        <v>256</v>
+      </c>
+      <c r="I890" s="5">
+        <v>5.4549999999999998E-3</v>
+      </c>
+      <c r="J890" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="891" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A891" s="5">
+        <v>10</v>
+      </c>
+      <c r="B891" s="5">
+        <v>5.7700000000000004E-4</v>
+      </c>
+      <c r="C891" s="5">
+        <v>2.6899999999999998E-4</v>
+      </c>
+      <c r="D891" s="5">
+        <v>4.8300000000000001E-3</v>
+      </c>
+      <c r="E891" s="5">
+        <v>1.804E-3</v>
+      </c>
+      <c r="F891" s="5">
+        <v>3.3599999999999998E-4</v>
+      </c>
+      <c r="G891" s="5">
+        <v>1.8799999999999999E-4</v>
+      </c>
+      <c r="H891" s="5">
+        <v>256</v>
+      </c>
+      <c r="I891" s="5">
+        <v>5.744E-3</v>
+      </c>
+      <c r="J891" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="892" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A892" s="5">
+        <v>12</v>
+      </c>
+      <c r="B892" s="5">
+        <v>6.2E-4</v>
+      </c>
+      <c r="C892" s="5">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="D892" s="5">
+        <v>3.715E-3</v>
+      </c>
+      <c r="E892" s="5">
+        <v>4.1999999999999998E-5</v>
+      </c>
+      <c r="F892" s="5">
+        <v>5.04E-4</v>
+      </c>
+      <c r="G892" s="5">
+        <v>1.07E-4</v>
+      </c>
+      <c r="H892" s="5">
+        <v>256</v>
+      </c>
+      <c r="I892" s="5">
+        <v>4.8390000000000004E-3</v>
+      </c>
+      <c r="J892" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="893" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A893" s="5">
+        <v>13</v>
+      </c>
+      <c r="B893" s="5">
+        <v>7.2000000000000005E-4</v>
+      </c>
+      <c r="C893" s="5">
+        <v>1.6799999999999999E-4</v>
+      </c>
+      <c r="D893" s="5">
+        <v>4.2919999999999998E-3</v>
+      </c>
+      <c r="E893" s="5">
+        <v>6.3900000000000003E-4</v>
+      </c>
+      <c r="F893" s="5">
+        <v>5.1699999999999999E-4</v>
+      </c>
+      <c r="G893" s="5">
+        <v>8.8999999999999995E-5</v>
+      </c>
+      <c r="H893" s="5">
+        <v>256</v>
+      </c>
+      <c r="I893" s="5">
+        <v>5.5290000000000001E-3</v>
+      </c>
+      <c r="J893" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="894" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A894" s="5">
         <v>16</v>
       </c>
-      <c r="B882" s="3"/>
-      <c r="C882" s="3"/>
-      <c r="D882" s="3"/>
-      <c r="E882" s="3"/>
-      <c r="F882" s="3"/>
-      <c r="G882" s="3"/>
-      <c r="H882" s="3"/>
-      <c r="I882" s="3"/>
-      <c r="J882" s="3"/>
+      <c r="B894" s="5">
+        <v>5.5400000000000002E-4</v>
+      </c>
+      <c r="C894" s="5">
+        <v>2.1000000000000001E-4</v>
+      </c>
+      <c r="D894" s="5">
+        <v>5.2129999999999998E-3</v>
+      </c>
+      <c r="E894" s="5">
+        <v>2.3939999999999999E-3</v>
+      </c>
+      <c r="F894" s="5">
+        <v>3.0400000000000002E-4</v>
+      </c>
+      <c r="G894" s="5">
+        <v>1.17E-4</v>
+      </c>
+      <c r="H894" s="5">
+        <v>256</v>
+      </c>
+      <c r="I894" s="5">
+        <v>6.0720000000000001E-3</v>
+      </c>
+      <c r="J894" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="895" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A895" s="5">
+        <v>18</v>
+      </c>
+      <c r="B895" s="5">
+        <v>4.8200000000000001E-4</v>
+      </c>
+      <c r="C895" s="5">
+        <v>2.31E-4</v>
+      </c>
+      <c r="D895" s="5">
+        <v>3.4129999999999998E-3</v>
+      </c>
+      <c r="E895" s="5">
+        <v>3.1000000000000001E-5</v>
+      </c>
+      <c r="F895" s="5">
+        <v>1.4200000000000001E-4</v>
+      </c>
+      <c r="G895" s="5">
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="H895" s="5">
+        <v>256</v>
+      </c>
+      <c r="I895" s="5">
+        <v>4.0369999999999998E-3</v>
+      </c>
+      <c r="J895" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="896" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A896" s="5">
+        <v>21</v>
+      </c>
+      <c r="B896" s="5">
+        <v>3.4200000000000002E-4</v>
+      </c>
+      <c r="C896" s="5">
+        <v>1.13E-4</v>
+      </c>
+      <c r="D896" s="5">
+        <v>4.3220000000000003E-3</v>
+      </c>
+      <c r="E896" s="5">
+        <v>1.217E-3</v>
+      </c>
+      <c r="F896" s="5">
+        <v>1.4899999999999999E-4</v>
+      </c>
+      <c r="G896" s="5">
+        <v>1.1E-5</v>
+      </c>
+      <c r="H896" s="5">
+        <v>256</v>
+      </c>
+      <c r="I896" s="5">
+        <v>4.8129999999999996E-3</v>
+      </c>
+      <c r="J896" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="897" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A897" s="5">
+        <v>24</v>
+      </c>
+      <c r="B897" s="5">
+        <v>5.4299999999999997E-4</v>
+      </c>
+      <c r="C897" s="5">
+        <v>3.8299999999999999E-4</v>
+      </c>
+      <c r="D897" s="5">
+        <v>4.045E-3</v>
+      </c>
+      <c r="E897" s="5">
+        <v>9.0300000000000005E-4</v>
+      </c>
+      <c r="F897" s="5">
+        <v>1.4300000000000001E-4</v>
+      </c>
+      <c r="G897" s="5">
+        <v>3.1999999999999999E-5</v>
+      </c>
+      <c r="H897" s="5">
+        <v>256</v>
+      </c>
+      <c r="I897" s="5">
+        <v>4.731E-3</v>
+      </c>
+      <c r="J897" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="898" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A898" s="5">
+        <v>27</v>
+      </c>
+      <c r="B898" s="5">
+        <v>1.155E-3</v>
+      </c>
+      <c r="C898" s="5">
+        <v>1.145E-3</v>
+      </c>
+      <c r="D898" s="5">
+        <v>3.5040000000000002E-3</v>
+      </c>
+      <c r="E898" s="5">
+        <v>1.5300000000000001E-4</v>
+      </c>
+      <c r="F898" s="5">
+        <v>1.3100000000000001E-4</v>
+      </c>
+      <c r="G898" s="5">
+        <v>1.1E-5</v>
+      </c>
+      <c r="H898" s="5">
+        <v>256</v>
+      </c>
+      <c r="I898" s="5">
+        <v>4.7889999999999999E-3</v>
+      </c>
+      <c r="J898" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="899" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A899" s="5">
+        <v>32</v>
+      </c>
+      <c r="B899" s="5">
+        <v>4.2499999999999998E-4</v>
+      </c>
+      <c r="C899" s="5">
+        <v>2.4899999999999998E-4</v>
+      </c>
+      <c r="D899" s="5">
+        <v>4.0810000000000004E-3</v>
+      </c>
+      <c r="E899" s="5">
+        <v>9.5600000000000004E-4</v>
+      </c>
+      <c r="F899" s="5">
+        <v>1.44E-4</v>
+      </c>
+      <c r="G899" s="5">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="H899" s="5">
+        <v>256</v>
+      </c>
+      <c r="I899" s="5">
+        <v>4.6499999999999996E-3</v>
+      </c>
+      <c r="J899" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="900" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A900" s="5">
+        <v>36</v>
+      </c>
+      <c r="B900" s="5">
+        <v>6.6299999999999996E-4</v>
+      </c>
+      <c r="C900" s="5">
+        <v>1.3200000000000001E-4</v>
+      </c>
+      <c r="D900" s="5">
+        <v>4.4339999999999996E-3</v>
+      </c>
+      <c r="E900" s="5">
+        <v>1.0120000000000001E-3</v>
+      </c>
+      <c r="F900" s="5">
+        <v>5.3300000000000005E-4</v>
+      </c>
+      <c r="G900" s="5">
+        <v>1.03E-4</v>
+      </c>
+      <c r="H900" s="5">
+        <v>256</v>
+      </c>
+      <c r="I900" s="5">
+        <v>5.6299999999999996E-3</v>
+      </c>
+      <c r="J900" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="901" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A901" s="5">
+        <v>42</v>
+      </c>
+      <c r="B901" s="5">
+        <v>5.8299999999999997E-4</v>
+      </c>
+      <c r="C901" s="5">
+        <v>1.3300000000000001E-4</v>
+      </c>
+      <c r="D901" s="5">
+        <v>3.5799999999999998E-3</v>
+      </c>
+      <c r="E901" s="5">
+        <v>1.45E-4</v>
+      </c>
+      <c r="F901" s="5">
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="G901" s="5">
+        <v>1.7799999999999999E-4</v>
+      </c>
+      <c r="H901" s="5">
+        <v>256</v>
+      </c>
+      <c r="I901" s="5">
+        <v>4.5040000000000002E-3</v>
+      </c>
+      <c r="J901" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="902" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A902" s="5">
+        <v>48</v>
+      </c>
+      <c r="B902" s="5">
+        <v>1.08E-3</v>
+      </c>
+      <c r="C902" s="5">
+        <v>1.073E-3</v>
+      </c>
+      <c r="D902" s="5">
+        <v>3.558E-3</v>
+      </c>
+      <c r="E902" s="5">
+        <v>1.21E-4</v>
+      </c>
+      <c r="F902" s="5">
+        <v>2.32E-4</v>
+      </c>
+      <c r="G902" s="5">
+        <v>4.6E-5</v>
+      </c>
+      <c r="H902" s="5">
+        <v>256</v>
+      </c>
+      <c r="I902" s="5">
+        <v>4.8700000000000002E-3</v>
+      </c>
+      <c r="J902" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="903" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A903" s="5">
+        <v>55</v>
+      </c>
+      <c r="B903" s="5">
+        <v>1.142E-3</v>
+      </c>
+      <c r="C903" s="5">
+        <v>5.2999999999999998E-4</v>
+      </c>
+      <c r="D903" s="5">
+        <v>3.7420000000000001E-3</v>
+      </c>
+      <c r="E903" s="5">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="F903" s="5">
+        <v>5.2999999999999998E-4</v>
+      </c>
+      <c r="G903" s="5">
+        <v>5.5000000000000002E-5</v>
+      </c>
+      <c r="H903" s="5">
+        <v>256</v>
+      </c>
+      <c r="I903" s="5">
+        <v>5.4140000000000004E-3</v>
+      </c>
+      <c r="J903" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="904" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A904" s="5">
+        <v>64</v>
+      </c>
+      <c r="B904" s="5">
+        <v>5.53E-4</v>
+      </c>
+      <c r="C904" s="5">
+        <v>8.8999999999999995E-5</v>
+      </c>
+      <c r="D904" s="5">
+        <v>4.437E-3</v>
+      </c>
+      <c r="E904" s="5">
+        <v>6.8900000000000005E-4</v>
+      </c>
+      <c r="F904" s="5">
+        <v>5.2400000000000005E-4</v>
+      </c>
+      <c r="G904" s="5">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="H904" s="5">
+        <v>256</v>
+      </c>
+      <c r="I904" s="5">
+        <v>5.5129999999999997E-3</v>
+      </c>
+      <c r="J904" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="905" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A905" s="5">
+        <v>73</v>
+      </c>
+      <c r="B905" s="5">
+        <v>6.2E-4</v>
+      </c>
+      <c r="C905" s="5">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="D905" s="5">
+        <v>4.2919999999999998E-3</v>
+      </c>
+      <c r="E905" s="5">
+        <v>8.8500000000000004E-4</v>
+      </c>
+      <c r="F905" s="5">
+        <v>5.4500000000000002E-4</v>
+      </c>
+      <c r="G905" s="5">
+        <v>1.2300000000000001E-4</v>
+      </c>
+      <c r="H905" s="5">
+        <v>256</v>
+      </c>
+      <c r="I905" s="5">
+        <v>5.457E-3</v>
+      </c>
+      <c r="J905" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="906" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A906" s="5">
+        <v>84</v>
+      </c>
+      <c r="B906" s="5">
+        <v>5.2999999999999998E-4</v>
+      </c>
+      <c r="C906" s="5">
+        <v>1.7200000000000001E-4</v>
+      </c>
+      <c r="D906" s="5">
+        <v>4.0870000000000004E-3</v>
+      </c>
+      <c r="E906" s="5">
+        <v>2.0699999999999999E-4</v>
+      </c>
+      <c r="F906" s="5">
+        <v>5.2300000000000003E-4</v>
+      </c>
+      <c r="G906" s="5">
+        <v>4.6999999999999997E-5</v>
+      </c>
+      <c r="H906" s="5">
+        <v>256</v>
+      </c>
+      <c r="I906" s="5">
+        <v>5.1399999999999996E-3</v>
+      </c>
+      <c r="J906" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="907" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A907" s="5">
+        <v>97</v>
+      </c>
+      <c r="B907" s="5">
+        <v>5.2499999999999997E-4</v>
+      </c>
+      <c r="C907" s="5">
+        <v>5.5999999999999999E-5</v>
+      </c>
+      <c r="D907" s="5">
+        <v>3.5990000000000002E-3</v>
+      </c>
+      <c r="E907" s="5">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="F907" s="5">
+        <v>3.0400000000000002E-4</v>
+      </c>
+      <c r="G907" s="5">
+        <v>1.3100000000000001E-4</v>
+      </c>
+      <c r="H907" s="5">
+        <v>256</v>
+      </c>
+      <c r="I907" s="5">
+        <v>4.4279999999999996E-3</v>
+      </c>
+      <c r="J907" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="908" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A908" s="5">
+        <v>111</v>
+      </c>
+      <c r="B908" s="5">
+        <v>1.1169999999999999E-3</v>
+      </c>
+      <c r="C908" s="5">
+        <v>3.2299999999999999E-4</v>
+      </c>
+      <c r="D908" s="5">
+        <v>4.0990000000000002E-3</v>
+      </c>
+      <c r="E908" s="5">
+        <v>3.8200000000000002E-4</v>
+      </c>
+      <c r="F908" s="5">
+        <v>4.7399999999999997E-4</v>
+      </c>
+      <c r="G908" s="5">
+        <v>6.7999999999999999E-5</v>
+      </c>
+      <c r="H908" s="5">
+        <v>256</v>
+      </c>
+      <c r="I908" s="5">
+        <v>5.6899999999999997E-3</v>
+      </c>
+      <c r="J908" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="909" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A909" s="5">
+        <v>128</v>
+      </c>
+      <c r="B909" s="5">
+        <v>8.2200000000000003E-4</v>
+      </c>
+      <c r="C909" s="5">
+        <v>2.02E-4</v>
+      </c>
+      <c r="D909" s="5">
+        <v>4.1840000000000002E-3</v>
+      </c>
+      <c r="E909" s="5">
+        <v>7.3800000000000005E-4</v>
+      </c>
+      <c r="F909" s="5">
+        <v>4.7600000000000002E-4</v>
+      </c>
+      <c r="G909" s="5">
+        <v>7.4999999999999993E-5</v>
+      </c>
+      <c r="H909" s="5">
+        <v>256</v>
+      </c>
+      <c r="I909" s="5">
+        <v>5.4819999999999999E-3</v>
+      </c>
+      <c r="J909" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="910" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A910" s="5">
+        <v>147</v>
+      </c>
+      <c r="B910" s="5">
+        <v>1.011E-3</v>
+      </c>
+      <c r="C910" s="5">
+        <v>3.5E-4</v>
+      </c>
+      <c r="D910" s="5">
+        <v>3.676E-3</v>
+      </c>
+      <c r="E910" s="5">
+        <v>3.8999999999999999E-5</v>
+      </c>
+      <c r="F910" s="5">
+        <v>4.35E-4</v>
+      </c>
+      <c r="G910" s="5">
+        <v>4.3000000000000002E-5</v>
+      </c>
+      <c r="H910" s="5">
+        <v>256</v>
+      </c>
+      <c r="I910" s="5">
+        <v>5.1219999999999998E-3</v>
+      </c>
+      <c r="J910" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="911" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A911" s="5">
+        <v>168</v>
+      </c>
+      <c r="B911" s="5">
+        <v>1.439E-3</v>
+      </c>
+      <c r="C911" s="5">
+        <v>1.0369999999999999E-3</v>
+      </c>
+      <c r="D911" s="5">
+        <v>3.9029999999999998E-3</v>
+      </c>
+      <c r="E911" s="5">
+        <v>2.02E-4</v>
+      </c>
+      <c r="F911" s="5">
+        <v>5.1500000000000005E-4</v>
+      </c>
+      <c r="G911" s="5">
+        <v>5.7000000000000003E-5</v>
+      </c>
+      <c r="H911" s="5">
+        <v>256</v>
+      </c>
+      <c r="I911" s="5">
+        <v>5.8570000000000002E-3</v>
+      </c>
+      <c r="J911" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="912" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A912" s="5">
+        <v>194</v>
+      </c>
+      <c r="B912" s="5">
+        <v>3.4900000000000003E-4</v>
+      </c>
+      <c r="C912" s="5">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="D912" s="5">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="E912" s="5">
+        <v>7.0100000000000002E-4</v>
+      </c>
+      <c r="F912" s="5">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="G912" s="5">
+        <v>1.3300000000000001E-4</v>
+      </c>
+      <c r="H912" s="5">
+        <v>256</v>
+      </c>
+      <c r="I912" s="5">
+        <v>4.6979999999999999E-3</v>
+      </c>
+      <c r="J912" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="913" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A913" s="5">
+        <v>222</v>
+      </c>
+      <c r="B913" s="5">
+        <v>4.0900000000000002E-4</v>
+      </c>
+      <c r="C913" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="D913" s="5">
+        <v>4.4520000000000002E-3</v>
+      </c>
+      <c r="E913" s="5">
+        <v>1.333E-3</v>
+      </c>
+      <c r="F913" s="5">
+        <v>2.8600000000000001E-4</v>
+      </c>
+      <c r="G913" s="5">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="H913" s="5">
+        <v>256</v>
+      </c>
+      <c r="I913" s="5">
+        <v>5.1469999999999997E-3</v>
+      </c>
+      <c r="J913" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="914" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A914" s="5">
+        <v>256</v>
+      </c>
+      <c r="B914" s="5">
+        <v>1.1670000000000001E-3</v>
+      </c>
+      <c r="C914" s="5">
+        <v>3.3199999999999999E-4</v>
+      </c>
+      <c r="D914" s="5">
+        <v>4.241E-3</v>
+      </c>
+      <c r="E914" s="5">
+        <v>8.92E-4</v>
+      </c>
+      <c r="F914" s="5">
+        <v>4.4700000000000002E-4</v>
+      </c>
+      <c r="G914" s="5">
+        <v>9.7E-5</v>
+      </c>
+      <c r="H914" s="5">
+        <v>256</v>
+      </c>
+      <c r="I914" s="5">
+        <v>5.855E-3</v>
+      </c>
+      <c r="J914" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="915" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A915" s="5">
+        <v>294</v>
+      </c>
+      <c r="B915" s="5">
+        <v>1.1980000000000001E-3</v>
+      </c>
+      <c r="C915" s="5">
+        <v>6.2100000000000002E-4</v>
+      </c>
+      <c r="D915" s="5">
+        <v>3.7859999999999999E-3</v>
+      </c>
+      <c r="E915" s="5">
+        <v>9.2999999999999997E-5</v>
+      </c>
+      <c r="F915" s="5">
+        <v>4.4999999999999999E-4</v>
+      </c>
+      <c r="G915" s="5">
+        <v>6.3999999999999997E-5</v>
+      </c>
+      <c r="H915" s="5">
+        <v>256</v>
+      </c>
+      <c r="I915" s="5">
+        <v>5.4339999999999996E-3</v>
+      </c>
+      <c r="J915" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="916" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A916" s="5">
+        <v>337</v>
+      </c>
+      <c r="B916" s="5">
+        <v>7.4299999999999995E-4</v>
+      </c>
+      <c r="C916" s="5">
+        <v>1.0900000000000001E-4</v>
+      </c>
+      <c r="D916" s="5">
+        <v>4.3049999999999998E-3</v>
+      </c>
+      <c r="E916" s="5">
+        <v>8.3500000000000002E-4</v>
+      </c>
+      <c r="F916" s="5">
+        <v>6.1600000000000001E-4</v>
+      </c>
+      <c r="G916" s="5">
+        <v>1.37E-4</v>
+      </c>
+      <c r="H916" s="5">
+        <v>256</v>
+      </c>
+      <c r="I916" s="5">
+        <v>5.6639999999999998E-3</v>
+      </c>
+      <c r="J916" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="917" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A917" s="5">
+        <v>388</v>
+      </c>
+      <c r="B917" s="5">
+        <v>1.4630000000000001E-3</v>
+      </c>
+      <c r="C917" s="5">
+        <v>8.3299999999999997E-4</v>
+      </c>
+      <c r="D917" s="5">
+        <v>3.8070000000000001E-3</v>
+      </c>
+      <c r="E917" s="5">
+        <v>1.35E-4</v>
+      </c>
+      <c r="F917" s="5">
+        <v>4.26E-4</v>
+      </c>
+      <c r="G917" s="5">
+        <v>1.5200000000000001E-4</v>
+      </c>
+      <c r="H917" s="5">
+        <v>256</v>
+      </c>
+      <c r="I917" s="5">
+        <v>5.6959999999999997E-3</v>
+      </c>
+      <c r="J917" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="918" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A918" s="5">
+        <v>445</v>
+      </c>
+      <c r="B918" s="5">
+        <v>7.3099999999999999E-4</v>
+      </c>
+      <c r="C918" s="5">
+        <v>1.2E-4</v>
+      </c>
+      <c r="D918" s="5">
+        <v>4.2859999999999999E-3</v>
+      </c>
+      <c r="E918" s="5">
+        <v>8.4900000000000004E-4</v>
+      </c>
+      <c r="F918" s="5">
+        <v>5.1000000000000004E-4</v>
+      </c>
+      <c r="G918" s="5">
+        <v>4.8999999999999998E-5</v>
+      </c>
+      <c r="H918" s="5">
+        <v>256</v>
+      </c>
+      <c r="I918" s="5">
+        <v>5.5269999999999998E-3</v>
+      </c>
+      <c r="J918" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="919" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A919" s="5">
+        <v>512</v>
+      </c>
+      <c r="B919" s="5">
+        <v>1.3290000000000001E-3</v>
+      </c>
+      <c r="C919" s="5">
+        <v>9.5600000000000004E-4</v>
+      </c>
+      <c r="D919" s="5">
+        <v>3.803E-3</v>
+      </c>
+      <c r="E919" s="5">
+        <v>1.76E-4</v>
+      </c>
+      <c r="F919" s="5">
+        <v>4.7399999999999997E-4</v>
+      </c>
+      <c r="G919" s="5">
+        <v>7.7000000000000001E-5</v>
+      </c>
+      <c r="H919" s="5">
+        <v>256</v>
+      </c>
+      <c r="I919" s="5">
+        <v>5.6059999999999999E-3</v>
+      </c>
+      <c r="J919" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="920" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A920" s="5">
+        <v>588</v>
+      </c>
+      <c r="B920" s="5">
+        <v>1.042E-3</v>
+      </c>
+      <c r="C920" s="5">
+        <v>6.4700000000000001E-4</v>
+      </c>
+      <c r="D920" s="5">
+        <v>4.5580000000000004E-3</v>
+      </c>
+      <c r="E920" s="5">
+        <v>1.341E-3</v>
+      </c>
+      <c r="F920" s="5">
+        <v>4.5199999999999998E-4</v>
+      </c>
+      <c r="G920" s="5">
+        <v>2.5799999999999998E-4</v>
+      </c>
+      <c r="H920" s="5">
+        <v>256</v>
+      </c>
+      <c r="I920" s="5">
+        <v>6.0520000000000001E-3</v>
+      </c>
+      <c r="J920" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="921" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A921" s="5">
+        <v>675</v>
+      </c>
+      <c r="B921" s="5">
+        <v>1.4790000000000001E-3</v>
+      </c>
+      <c r="C921" s="5">
+        <v>8.5400000000000005E-4</v>
+      </c>
+      <c r="D921" s="5">
+        <v>4.0959999999999998E-3</v>
+      </c>
+      <c r="E921" s="5">
+        <v>5.6800000000000004E-4</v>
+      </c>
+      <c r="F921" s="5">
+        <v>4.8999999999999998E-4</v>
+      </c>
+      <c r="G921" s="5">
+        <v>1.05E-4</v>
+      </c>
+      <c r="H921" s="5">
+        <v>256</v>
+      </c>
+      <c r="I921" s="5">
+        <v>6.0639999999999999E-3</v>
+      </c>
+      <c r="J921" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="922" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A922" s="5">
+        <v>776</v>
+      </c>
+      <c r="B922" s="5">
+        <v>5.2300000000000003E-4</v>
+      </c>
+      <c r="C922" s="5">
+        <v>7.8999999999999996E-5</v>
+      </c>
+      <c r="D922" s="5">
+        <v>4.0049999999999999E-3</v>
+      </c>
+      <c r="E922" s="5">
+        <v>5.5500000000000005E-4</v>
+      </c>
+      <c r="F922" s="5">
+        <v>3.3599999999999998E-4</v>
+      </c>
+      <c r="G922" s="5">
+        <v>3.4E-5</v>
+      </c>
+      <c r="H922" s="5">
+        <v>256</v>
+      </c>
+      <c r="I922" s="5">
+        <v>4.8630000000000001E-3</v>
+      </c>
+      <c r="J922" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="923" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A923" s="5">
+        <v>891</v>
+      </c>
+      <c r="B923" s="5">
+        <v>1.377E-3</v>
+      </c>
+      <c r="C923" s="5">
+        <v>1.1180000000000001E-3</v>
+      </c>
+      <c r="D923" s="5">
+        <v>3.7399999999999998E-3</v>
+      </c>
+      <c r="E923" s="5">
+        <v>1.83E-4</v>
+      </c>
+      <c r="F923" s="5">
+        <v>3.4900000000000003E-4</v>
+      </c>
+      <c r="G923" s="5">
+        <v>2.1800000000000001E-4</v>
+      </c>
+      <c r="H923" s="5">
+        <v>256</v>
+      </c>
+      <c r="I923" s="5">
+        <v>5.4660000000000004E-3</v>
+      </c>
+      <c r="J923" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="924" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A924" s="5">
+        <v>1024</v>
+      </c>
+      <c r="B924" s="5">
+        <v>6.4700000000000001E-4</v>
+      </c>
+      <c r="C924" s="5">
+        <v>1.07E-4</v>
+      </c>
+      <c r="D924" s="5">
+        <v>3.6150000000000002E-3</v>
+      </c>
+      <c r="E924" s="5">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="F924" s="5">
+        <v>5.0799999999999999E-4</v>
+      </c>
+      <c r="G924" s="5">
+        <v>1.4E-5</v>
+      </c>
+      <c r="H924" s="5">
+        <v>256</v>
+      </c>
+      <c r="I924" s="5">
+        <v>4.7699999999999999E-3</v>
+      </c>
+      <c r="J924" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="925" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A925" s="5">
+        <v>1176</v>
+      </c>
+      <c r="B925" s="5">
+        <v>1.253E-3</v>
+      </c>
+      <c r="C925" s="5">
+        <v>6.8400000000000004E-4</v>
+      </c>
+      <c r="D925" s="5">
+        <v>3.8159999999999999E-3</v>
+      </c>
+      <c r="E925" s="5">
+        <v>1.73E-4</v>
+      </c>
+      <c r="F925" s="5">
+        <v>4.4299999999999998E-4</v>
+      </c>
+      <c r="G925" s="5">
+        <v>1.02E-4</v>
+      </c>
+      <c r="H925" s="5">
+        <v>256</v>
+      </c>
+      <c r="I925" s="5">
+        <v>5.5120000000000004E-3</v>
+      </c>
+      <c r="J925" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="926" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A926" s="5">
+        <v>1351</v>
+      </c>
+      <c r="B926" s="5">
+        <v>9.8700000000000003E-4</v>
+      </c>
+      <c r="C926" s="5">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="D926" s="5">
+        <v>4.2579999999999996E-3</v>
+      </c>
+      <c r="E926" s="5">
+        <v>8.3600000000000005E-4</v>
+      </c>
+      <c r="F926" s="5">
+        <v>4.95E-4</v>
+      </c>
+      <c r="G926" s="5">
+        <v>5.8E-5</v>
+      </c>
+      <c r="H926" s="5">
+        <v>256</v>
+      </c>
+      <c r="I926" s="5">
+        <v>5.7400000000000003E-3</v>
+      </c>
+      <c r="J926" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="927" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A927" s="5">
+        <v>1552</v>
+      </c>
+      <c r="B927" s="5">
+        <v>1.3649999999999999E-3</v>
+      </c>
+      <c r="C927" s="5">
+        <v>8.5999999999999998E-4</v>
+      </c>
+      <c r="D927" s="5">
+        <v>3.823E-3</v>
+      </c>
+      <c r="E927" s="5">
+        <v>2.0599999999999999E-4</v>
+      </c>
+      <c r="F927" s="5">
+        <v>4.4499999999999997E-4</v>
+      </c>
+      <c r="G927" s="5">
+        <v>6.6000000000000005E-5</v>
+      </c>
+      <c r="H927" s="5">
+        <v>256</v>
+      </c>
+      <c r="I927" s="5">
+        <v>5.6340000000000001E-3</v>
+      </c>
+      <c r="J927" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="928" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A928" s="5">
+        <v>1782</v>
+      </c>
+      <c r="B928" s="5">
+        <v>1.088E-3</v>
+      </c>
+      <c r="C928" s="5">
+        <v>5.9900000000000003E-4</v>
+      </c>
+      <c r="D928" s="5">
+        <v>3.764E-3</v>
+      </c>
+      <c r="E928" s="5">
+        <v>1.1900000000000001E-4</v>
+      </c>
+      <c r="F928" s="5">
+        <v>5.8900000000000001E-4</v>
+      </c>
+      <c r="G928" s="5">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="H928" s="5">
+        <v>256</v>
+      </c>
+      <c r="I928" s="5">
+        <v>5.4409999999999997E-3</v>
+      </c>
+      <c r="J928" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="929" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A929" s="5">
+        <v>2048</v>
+      </c>
+      <c r="B929" s="5">
+        <v>1.735E-3</v>
+      </c>
+      <c r="C929" s="5">
+        <v>1.786E-3</v>
+      </c>
+      <c r="D929" s="5">
+        <v>3.7190000000000001E-3</v>
+      </c>
+      <c r="E929" s="5">
+        <v>1.45E-4</v>
+      </c>
+      <c r="F929" s="5">
+        <v>3.6600000000000001E-4</v>
+      </c>
+      <c r="G929" s="5">
+        <v>1.1E-4</v>
+      </c>
+      <c r="H929" s="5">
+        <v>256</v>
+      </c>
+      <c r="I929" s="5">
+        <v>5.8199999999999997E-3</v>
+      </c>
+      <c r="J929" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="930" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A930" s="5">
+        <v>2352</v>
+      </c>
+      <c r="B930" s="5">
+        <v>8.3000000000000001E-4</v>
+      </c>
+      <c r="C930" s="5">
+        <v>1.73E-4</v>
+      </c>
+      <c r="D930" s="5">
+        <v>4.2050000000000004E-3</v>
+      </c>
+      <c r="E930" s="5">
+        <v>6.9099999999999999E-4</v>
+      </c>
+      <c r="F930" s="5">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G930" s="5">
+        <v>1.93E-4</v>
+      </c>
+      <c r="H930" s="5">
+        <v>256</v>
+      </c>
+      <c r="I930" s="5">
+        <v>5.4349999999999997E-3</v>
+      </c>
+      <c r="J930" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="931" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A931" s="5">
+        <v>2702</v>
+      </c>
+      <c r="B931" s="5">
+        <v>7.36E-4</v>
+      </c>
+      <c r="C931" s="5">
+        <v>1.6699999999999999E-4</v>
+      </c>
+      <c r="D931" s="5">
+        <v>3.9779999999999998E-3</v>
+      </c>
+      <c r="E931" s="5">
+        <v>4.6299999999999998E-4</v>
+      </c>
+      <c r="F931" s="5">
+        <v>3.9599999999999998E-4</v>
+      </c>
+      <c r="G931" s="5">
+        <v>9.2999999999999997E-5</v>
+      </c>
+      <c r="H931" s="5">
+        <v>256</v>
+      </c>
+      <c r="I931" s="5">
+        <v>5.1089999999999998E-3</v>
+      </c>
+      <c r="J931" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="932" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A932" s="5">
+        <v>3104</v>
+      </c>
+      <c r="B932" s="5">
+        <v>6.0599999999999998E-4</v>
+      </c>
+      <c r="C932" s="5">
+        <v>1.7899999999999999E-4</v>
+      </c>
+      <c r="D932" s="5">
+        <v>3.973E-3</v>
+      </c>
+      <c r="E932" s="5">
+        <v>3.9899999999999999E-4</v>
+      </c>
+      <c r="F932" s="5">
+        <v>6.6E-4</v>
+      </c>
+      <c r="G932" s="5">
+        <v>5.5999999999999999E-5</v>
+      </c>
+      <c r="H932" s="5">
+        <v>256</v>
+      </c>
+      <c r="I932" s="5">
+        <v>5.2399999999999999E-3</v>
+      </c>
+      <c r="J932" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="933" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A933" s="5">
+        <v>3565</v>
+      </c>
+      <c r="B933" s="5">
+        <v>7.76E-4</v>
+      </c>
+      <c r="C933" s="5">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="D933" s="5">
+        <v>4.2700000000000004E-3</v>
+      </c>
+      <c r="E933" s="5">
+        <v>8.4800000000000001E-4</v>
+      </c>
+      <c r="F933" s="5">
+        <v>6.1200000000000002E-4</v>
+      </c>
+      <c r="G933" s="5">
+        <v>4.6E-5</v>
+      </c>
+      <c r="H933" s="5">
+        <v>256</v>
+      </c>
+      <c r="I933" s="5">
+        <v>5.6579999999999998E-3</v>
+      </c>
+      <c r="J933" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="934" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A934" s="5">
+        <v>4096</v>
+      </c>
+      <c r="B934" s="5">
+        <v>8.12E-4</v>
+      </c>
+      <c r="C934" s="5">
+        <v>6.7500000000000004E-4</v>
+      </c>
+      <c r="D934" s="5">
+        <v>3.5149999999999999E-3</v>
+      </c>
+      <c r="E934" s="5">
+        <v>1.5899999999999999E-4</v>
+      </c>
+      <c r="F934" s="5">
+        <v>1.95E-4</v>
+      </c>
+      <c r="G934" s="5">
+        <v>2.6999999999999999E-5</v>
+      </c>
+      <c r="H934" s="5">
+        <v>256</v>
+      </c>
+      <c r="I934" s="5">
+        <v>4.5230000000000001E-3</v>
+      </c>
+      <c r="J934" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="935" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A935" s="5">
+        <v>4705</v>
+      </c>
+      <c r="B935" s="5">
+        <v>7.2800000000000002E-4</v>
+      </c>
+      <c r="C935" s="5">
+        <v>1.4300000000000001E-4</v>
+      </c>
+      <c r="D935" s="5">
+        <v>4.8209999999999998E-3</v>
+      </c>
+      <c r="E935" s="5">
+        <v>1.812E-3</v>
+      </c>
+      <c r="F935" s="5">
+        <v>5.4500000000000002E-4</v>
+      </c>
+      <c r="G935" s="5">
+        <v>1.07E-4</v>
+      </c>
+      <c r="H935" s="5">
+        <v>256</v>
+      </c>
+      <c r="I935" s="5">
+        <v>6.0930000000000003E-3</v>
+      </c>
+      <c r="J935" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="936" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A936" s="5">
+        <v>5404</v>
+      </c>
+      <c r="B936" s="5">
+        <v>8.1099999999999998E-4</v>
+      </c>
+      <c r="C936" s="5">
+        <v>1.21E-4</v>
+      </c>
+      <c r="D936" s="5">
+        <v>3.9630000000000004E-3</v>
+      </c>
+      <c r="E936" s="5">
+        <v>5.1099999999999995E-4</v>
+      </c>
+      <c r="F936" s="5">
+        <v>6.3299999999999999E-4</v>
+      </c>
+      <c r="G936" s="5">
+        <v>9.2E-5</v>
+      </c>
+      <c r="H936" s="5">
+        <v>256</v>
+      </c>
+      <c r="I936" s="5">
+        <v>5.4070000000000003E-3</v>
+      </c>
+      <c r="J936" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="937" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A937" s="5">
+        <v>6208</v>
+      </c>
+      <c r="B937" s="5">
+        <v>7.54E-4</v>
+      </c>
+      <c r="C937" s="5">
+        <v>1.03E-4</v>
+      </c>
+      <c r="D937" s="5">
+        <v>4.3670000000000002E-3</v>
+      </c>
+      <c r="E937" s="5">
+        <v>1.206E-3</v>
+      </c>
+      <c r="F937" s="5">
+        <v>3.6699999999999998E-4</v>
+      </c>
+      <c r="G937" s="5">
+        <v>1.7799999999999999E-4</v>
+      </c>
+      <c r="H937" s="5">
+        <v>256</v>
+      </c>
+      <c r="I937" s="5">
+        <v>5.4869999999999997E-3</v>
+      </c>
+      <c r="J937" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="938" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A938" s="5">
+        <v>7131</v>
+      </c>
+      <c r="B938" s="5">
+        <v>6.8000000000000005E-4</v>
+      </c>
+      <c r="C938" s="5">
+        <v>1.01E-4</v>
+      </c>
+      <c r="D938" s="5">
+        <v>4.176E-3</v>
+      </c>
+      <c r="E938" s="5">
+        <v>8.6600000000000002E-4</v>
+      </c>
+      <c r="F938" s="5">
+        <v>4.8200000000000001E-4</v>
+      </c>
+      <c r="G938" s="5">
+        <v>9.2999999999999997E-5</v>
+      </c>
+      <c r="H938" s="5">
+        <v>256</v>
+      </c>
+      <c r="I938" s="5">
+        <v>5.3379999999999999E-3</v>
+      </c>
+      <c r="J938" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="939" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A939" s="5">
+        <v>8192</v>
+      </c>
+      <c r="B939" s="5">
+        <v>1.1039999999999999E-3</v>
+      </c>
+      <c r="C939" s="5">
+        <v>2.63E-4</v>
+      </c>
+      <c r="D939" s="5">
+        <v>3.6180000000000001E-3</v>
+      </c>
+      <c r="E939" s="5">
+        <v>5.7000000000000003E-5</v>
+      </c>
+      <c r="F939" s="5">
+        <v>4.5300000000000001E-4</v>
+      </c>
+      <c r="G939" s="5">
+        <v>5.5999999999999999E-5</v>
+      </c>
+      <c r="H939" s="5">
+        <v>256</v>
+      </c>
+      <c r="I939" s="5">
+        <v>5.1749999999999999E-3</v>
+      </c>
+      <c r="J939" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="940" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A940" s="5">
+        <v>9410</v>
+      </c>
+      <c r="B940" s="5">
+        <v>9.1600000000000004E-4</v>
+      </c>
+      <c r="C940" s="5">
+        <v>8.3999999999999995E-5</v>
+      </c>
+      <c r="D940" s="5">
+        <v>3.6340000000000001E-3</v>
+      </c>
+      <c r="E940" s="5">
+        <v>5.3999999999999998E-5</v>
+      </c>
+      <c r="F940" s="5">
+        <v>4.1599999999999997E-4</v>
+      </c>
+      <c r="G940" s="5">
+        <v>1.74E-4</v>
+      </c>
+      <c r="H940" s="5">
+        <v>256</v>
+      </c>
+      <c r="I940" s="5">
+        <v>4.9659999999999999E-3</v>
+      </c>
+      <c r="J940" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="941" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A941" s="5">
+        <v>10809</v>
+      </c>
+      <c r="B941" s="5">
+        <v>1.472E-3</v>
+      </c>
+      <c r="C941" s="5">
+        <v>8.9599999999999999E-4</v>
+      </c>
+      <c r="D941" s="5">
+        <v>3.6519999999999999E-3</v>
+      </c>
+      <c r="E941" s="5">
+        <v>1.11E-4</v>
+      </c>
+      <c r="F941" s="5">
+        <v>5.4900000000000001E-4</v>
+      </c>
+      <c r="G941" s="5">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="H941" s="5">
+        <v>256</v>
+      </c>
+      <c r="I941" s="5">
+        <v>5.6730000000000001E-3</v>
+      </c>
+      <c r="J941" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="942" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A942" s="5">
+        <v>12416</v>
+      </c>
+      <c r="B942" s="5">
+        <v>8.3799999999999999E-4</v>
+      </c>
+      <c r="C942" s="5">
+        <v>8.7999999999999998E-5</v>
+      </c>
+      <c r="D942" s="5">
+        <v>4.0619999999999996E-3</v>
+      </c>
+      <c r="E942" s="5">
+        <v>5.2300000000000003E-4</v>
+      </c>
+      <c r="F942" s="5">
+        <v>4.8700000000000002E-4</v>
+      </c>
+      <c r="G942" s="5">
+        <v>7.2000000000000002E-5</v>
+      </c>
+      <c r="H942" s="5">
+        <v>256</v>
+      </c>
+      <c r="I942" s="5">
+        <v>5.3860000000000002E-3</v>
+      </c>
+      <c r="J942" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="943" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A943" s="5">
+        <v>14263</v>
+      </c>
+      <c r="B943" s="5">
+        <v>7.1199999999999996E-4</v>
+      </c>
+      <c r="C943" s="5">
+        <v>9.7E-5</v>
+      </c>
+      <c r="D943" s="5">
+        <v>4.3410000000000002E-3</v>
+      </c>
+      <c r="E943" s="5">
+        <v>1.1329999999999999E-3</v>
+      </c>
+      <c r="F943" s="5">
+        <v>5.44E-4</v>
+      </c>
+      <c r="G943" s="5">
+        <v>8.8999999999999995E-5</v>
+      </c>
+      <c r="H943" s="5">
+        <v>256</v>
+      </c>
+      <c r="I943" s="5">
+        <v>5.5979999999999997E-3</v>
+      </c>
+      <c r="J943" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="944" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A944" s="5">
+        <v>16384</v>
+      </c>
+      <c r="B944" s="5">
+        <v>7.0799999999999997E-4</v>
+      </c>
+      <c r="C944" s="5">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="D944" s="5">
+        <v>3.9480000000000001E-3</v>
+      </c>
+      <c r="E944" s="5">
+        <v>6.7500000000000004E-4</v>
+      </c>
+      <c r="F944" s="5">
+        <v>5.13E-4</v>
+      </c>
+      <c r="G944" s="5">
+        <v>1.3200000000000001E-4</v>
+      </c>
+      <c r="H944" s="5">
+        <v>256</v>
+      </c>
+      <c r="I944" s="5">
+        <v>5.1700000000000001E-3</v>
+      </c>
+      <c r="J944" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="945" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A945" s="5">
+        <v>18820</v>
+      </c>
+      <c r="B945" s="5">
+        <v>7.7899999999999996E-4</v>
+      </c>
+      <c r="C945" s="5">
+        <v>1.2300000000000001E-4</v>
+      </c>
+      <c r="D945" s="5">
+        <v>4.2810000000000001E-3</v>
+      </c>
+      <c r="E945" s="5">
+        <v>1.3550000000000001E-3</v>
+      </c>
+      <c r="F945" s="5">
+        <v>4.2299999999999998E-4</v>
+      </c>
+      <c r="G945" s="5">
+        <v>1.6899999999999999E-4</v>
+      </c>
+      <c r="H945" s="5">
+        <v>256</v>
+      </c>
+      <c r="I945" s="5">
+        <v>5.4840000000000002E-3</v>
+      </c>
+      <c r="J945" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="946" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A946" s="5">
+        <v>21618</v>
+      </c>
+      <c r="B946" s="5">
+        <v>1.018E-3</v>
+      </c>
+      <c r="C946" s="5">
+        <v>2.1699999999999999E-4</v>
+      </c>
+      <c r="D946" s="5">
+        <v>3.3930000000000002E-3</v>
+      </c>
+      <c r="E946" s="5">
+        <v>8.2999999999999998E-5</v>
+      </c>
+      <c r="F946" s="5">
+        <v>5.6700000000000001E-4</v>
+      </c>
+      <c r="G946" s="5">
+        <v>4.1999999999999998E-5</v>
+      </c>
+      <c r="H946" s="5">
+        <v>256</v>
+      </c>
+      <c r="I946" s="5">
+        <v>4.9769999999999997E-3</v>
+      </c>
+      <c r="J946" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="947" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A947" s="5">
+        <v>24833</v>
+      </c>
+      <c r="B947" s="5">
+        <v>1.531E-3</v>
+      </c>
+      <c r="C947" s="5">
+        <v>1.2880000000000001E-3</v>
+      </c>
+      <c r="D947" s="5">
+        <v>3.467E-3</v>
+      </c>
+      <c r="E947" s="5">
+        <v>1.6699999999999999E-4</v>
+      </c>
+      <c r="F947" s="5">
+        <v>4.6200000000000001E-4</v>
+      </c>
+      <c r="G947" s="5">
+        <v>1.54E-4</v>
+      </c>
+      <c r="H947" s="5">
+        <v>256</v>
+      </c>
+      <c r="I947" s="5">
+        <v>5.4599999999999996E-3</v>
+      </c>
+      <c r="J947" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="948" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A948" s="5">
+        <v>28526</v>
+      </c>
+      <c r="B948" s="5">
+        <v>1.0430000000000001E-3</v>
+      </c>
+      <c r="C948" s="5">
+        <v>6.1700000000000004E-4</v>
+      </c>
+      <c r="D948" s="5">
+        <v>3.29E-3</v>
+      </c>
+      <c r="E948" s="5">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="F948" s="5">
+        <v>3.57E-4</v>
+      </c>
+      <c r="G948" s="5">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="H948" s="5">
+        <v>256</v>
+      </c>
+      <c r="I948" s="5">
+        <v>4.6889999999999996E-3</v>
+      </c>
+      <c r="J948" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="949" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A949" s="5">
+        <v>32768</v>
+      </c>
+      <c r="B949" s="5">
+        <v>3.2200000000000002E-4</v>
+      </c>
+      <c r="C949" s="5">
+        <v>1.03E-4</v>
+      </c>
+      <c r="D949" s="5">
+        <v>4.8919999999999996E-3</v>
+      </c>
+      <c r="E949" s="5">
+        <v>2.496E-3</v>
+      </c>
+      <c r="F949" s="5">
+        <v>3.8999999999999999E-4</v>
+      </c>
+      <c r="G949" s="5">
+        <v>1.8699999999999999E-4</v>
+      </c>
+      <c r="H949" s="5">
+        <v>256</v>
+      </c>
+      <c r="I949" s="5">
+        <v>5.6049999999999997E-3</v>
+      </c>
+      <c r="J949" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="950" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A950" s="5">
+        <v>37640</v>
+      </c>
+      <c r="B950" s="5">
+        <v>2.1930000000000001E-3</v>
+      </c>
+      <c r="C950" s="5">
+        <v>1.9959999999999999E-3</v>
+      </c>
+      <c r="D950" s="5">
+        <v>4.4640000000000001E-3</v>
+      </c>
+      <c r="E950" s="5">
+        <v>3.6200000000000002E-4</v>
+      </c>
+      <c r="F950" s="5">
+        <v>5.1099999999999995E-4</v>
+      </c>
+      <c r="G950" s="5">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="H950" s="5">
+        <v>256</v>
+      </c>
+      <c r="I950" s="5">
+        <v>7.1679999999999999E-3</v>
+      </c>
+      <c r="J950" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="951" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A951" s="5">
+        <v>43237</v>
+      </c>
+      <c r="B951" s="5">
+        <v>1.193E-3</v>
+      </c>
+      <c r="C951" s="5">
+        <v>4.7699999999999999E-4</v>
+      </c>
+      <c r="D951" s="5">
+        <v>4.1570000000000001E-3</v>
+      </c>
+      <c r="E951" s="5">
+        <v>1.47E-4</v>
+      </c>
+      <c r="F951" s="5">
+        <v>5.2300000000000003E-4</v>
+      </c>
+      <c r="G951" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="H951" s="5">
+        <v>256</v>
+      </c>
+      <c r="I951" s="5">
+        <v>5.8719999999999996E-3</v>
+      </c>
+      <c r="J951" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="952" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A952" s="5">
+        <v>49667</v>
+      </c>
+      <c r="B952" s="5">
+        <v>1.5839999999999999E-3</v>
+      </c>
+      <c r="C952" s="5">
+        <v>9.8799999999999995E-4</v>
+      </c>
+      <c r="D952" s="5">
+        <v>4.1949999999999999E-3</v>
+      </c>
+      <c r="E952" s="5">
+        <v>1.7699999999999999E-4</v>
+      </c>
+      <c r="F952" s="5">
+        <v>6.2799999999999998E-4</v>
+      </c>
+      <c r="G952" s="5">
+        <v>5.1999999999999997E-5</v>
+      </c>
+      <c r="H952" s="5">
+        <v>256</v>
+      </c>
+      <c r="I952" s="5">
+        <v>6.4070000000000004E-3</v>
+      </c>
+      <c r="J952" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="953" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A953" s="5">
+        <v>57052</v>
+      </c>
+      <c r="B953" s="5">
+        <v>1.1789999999999999E-3</v>
+      </c>
+      <c r="C953" s="5">
+        <v>2.9300000000000002E-4</v>
+      </c>
+      <c r="D953" s="5">
+        <v>4.2050000000000004E-3</v>
+      </c>
+      <c r="E953" s="5">
+        <v>9.5000000000000005E-5</v>
+      </c>
+      <c r="F953" s="5">
+        <v>7.2099999999999996E-4</v>
+      </c>
+      <c r="G953" s="5">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="H953" s="5">
+        <v>256</v>
+      </c>
+      <c r="I953" s="5">
+        <v>6.1040000000000001E-3</v>
+      </c>
+      <c r="J953" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="954" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A954" s="5">
+        <v>65536</v>
+      </c>
+      <c r="B954" s="5">
+        <v>6.7100000000000005E-4</v>
+      </c>
+      <c r="C954" s="5">
+        <v>7.3999999999999996E-5</v>
+      </c>
+      <c r="D954" s="5">
+        <v>4.7980000000000002E-3</v>
+      </c>
+      <c r="E954" s="5">
+        <v>1.0759999999999999E-3</v>
+      </c>
+      <c r="F954" s="5">
+        <v>7.1699999999999997E-4</v>
+      </c>
+      <c r="G954" s="5">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="H954" s="5">
+        <v>256</v>
+      </c>
+      <c r="I954" s="5">
+        <v>6.1859999999999997E-3</v>
+      </c>
+      <c r="J954" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="955" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A955" s="5">
+        <v>75281</v>
+      </c>
+      <c r="B955" s="5">
+        <v>1.369E-3</v>
+      </c>
+      <c r="C955" s="5">
+        <v>5.9699999999999998E-4</v>
+      </c>
+      <c r="D955" s="5">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="E955" s="5">
+        <v>1.83E-4</v>
+      </c>
+      <c r="F955" s="5">
+        <v>7.3200000000000001E-4</v>
+      </c>
+      <c r="G955" s="5">
+        <v>7.3999999999999996E-5</v>
+      </c>
+      <c r="H955" s="5">
+        <v>256</v>
+      </c>
+      <c r="I955" s="5">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="J955" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="956" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A956" s="5">
+        <v>86475</v>
+      </c>
+      <c r="B956" s="5">
+        <v>1.1919999999999999E-3</v>
+      </c>
+      <c r="C956" s="5">
+        <v>1.93E-4</v>
+      </c>
+      <c r="D956" s="5">
+        <v>4.3819999999999996E-3</v>
+      </c>
+      <c r="E956" s="5">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="F956" s="5">
+        <v>5.7600000000000001E-4</v>
+      </c>
+      <c r="G956" s="5">
+        <v>7.7000000000000001E-5</v>
+      </c>
+      <c r="H956" s="5">
+        <v>256</v>
+      </c>
+      <c r="I956" s="5">
+        <v>6.1510000000000002E-3</v>
+      </c>
+      <c r="J956" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="957" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A957" s="5">
+        <v>99334</v>
+      </c>
+      <c r="B957" s="5">
+        <v>1.2489999999999999E-3</v>
+      </c>
+      <c r="C957" s="5">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="D957" s="5">
+        <v>5.6020000000000002E-3</v>
+      </c>
+      <c r="E957" s="5">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="F957" s="5">
+        <v>7.9600000000000005E-4</v>
+      </c>
+      <c r="G957" s="5">
+        <v>2.6999999999999999E-5</v>
+      </c>
+      <c r="H957" s="5">
+        <v>256</v>
+      </c>
+      <c r="I957" s="5">
+        <v>7.6480000000000003E-3</v>
+      </c>
+      <c r="J957" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="958" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A958" s="5">
+        <v>114104</v>
+      </c>
+      <c r="B958" s="5">
+        <v>2.016E-3</v>
+      </c>
+      <c r="C958" s="5">
+        <v>1.237E-3</v>
+      </c>
+      <c r="D958" s="5">
+        <v>5.5059999999999996E-3</v>
+      </c>
+      <c r="E958" s="5">
+        <v>7.2000000000000002E-5</v>
+      </c>
+      <c r="F958" s="5">
+        <v>8.12E-4</v>
+      </c>
+      <c r="G958" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="H958" s="5">
+        <v>256</v>
+      </c>
+      <c r="I958" s="5">
+        <v>8.3330000000000001E-3</v>
+      </c>
+      <c r="J958" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="959" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A959" s="5">
+        <v>131072</v>
+      </c>
+      <c r="B959" s="5">
+        <v>7.0299999999999996E-4</v>
+      </c>
+      <c r="C959" s="5">
+        <v>1.21E-4</v>
+      </c>
+      <c r="D959" s="5">
+        <v>5.9439999999999996E-3</v>
+      </c>
+      <c r="E959" s="5">
+        <v>4.7199999999999998E-4</v>
+      </c>
+      <c r="F959" s="5">
+        <v>8.7900000000000001E-4</v>
+      </c>
+      <c r="G959" s="5">
+        <v>9.8999999999999994E-5</v>
+      </c>
+      <c r="H959" s="5">
+        <v>256</v>
+      </c>
+      <c r="I959" s="5">
+        <v>7.5259999999999997E-3</v>
+      </c>
+      <c r="J959" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="960" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A960" s="5">
+        <v>150562</v>
+      </c>
+      <c r="B960" s="5">
+        <v>1.3029999999999999E-3</v>
+      </c>
+      <c r="C960" s="5">
+        <v>1.3300000000000001E-4</v>
+      </c>
+      <c r="D960" s="5">
+        <v>6.6800000000000002E-3</v>
+      </c>
+      <c r="E960" s="5">
+        <v>9.3099999999999997E-4</v>
+      </c>
+      <c r="F960" s="5">
+        <v>8.9700000000000001E-4</v>
+      </c>
+      <c r="G960" s="5">
+        <v>6.7999999999999999E-5</v>
+      </c>
+      <c r="H960" s="5">
+        <v>256</v>
+      </c>
+      <c r="I960" s="5">
+        <v>8.8789999999999997E-3</v>
+      </c>
+      <c r="J960" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="961" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A961" s="5">
+        <v>172950</v>
+      </c>
+      <c r="B961" s="5">
+        <v>1.335E-3</v>
+      </c>
+      <c r="C961" s="5">
+        <v>8.8999999999999995E-5</v>
+      </c>
+      <c r="D961" s="5">
+        <v>8.2369999999999995E-3</v>
+      </c>
+      <c r="E961" s="5">
+        <v>3.77E-4</v>
+      </c>
+      <c r="F961" s="5">
+        <v>8.7399999999999999E-4</v>
+      </c>
+      <c r="G961" s="5">
+        <v>3.3000000000000003E-5</v>
+      </c>
+      <c r="H961" s="5">
+        <v>256</v>
+      </c>
+      <c r="I961" s="5">
+        <v>1.0444999999999999E-2</v>
+      </c>
+      <c r="J961" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="962" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A962" s="5">
+        <v>198668</v>
+      </c>
+      <c r="B962" s="5">
+        <v>1.3010000000000001E-3</v>
+      </c>
+      <c r="C962" s="5">
+        <v>2.8600000000000001E-4</v>
+      </c>
+      <c r="D962" s="5">
+        <v>8.829E-3</v>
+      </c>
+      <c r="E962" s="5">
+        <v>1.73E-4</v>
+      </c>
+      <c r="F962" s="5">
+        <v>8.7100000000000003E-4</v>
+      </c>
+      <c r="G962" s="5">
+        <v>1.12E-4</v>
+      </c>
+      <c r="H962" s="5">
+        <v>256</v>
+      </c>
+      <c r="I962" s="5">
+        <v>1.1001E-2</v>
+      </c>
+      <c r="J962" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="963" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A963" s="5">
+        <v>228209</v>
+      </c>
+      <c r="B963" s="5">
+        <v>1.3450000000000001E-3</v>
+      </c>
+      <c r="C963" s="5">
+        <v>9.7999999999999997E-5</v>
+      </c>
+      <c r="D963" s="5">
+        <v>8.5100000000000002E-3</v>
+      </c>
+      <c r="E963" s="5">
+        <v>1.5100000000000001E-4</v>
+      </c>
+      <c r="F963" s="5">
+        <v>1.0349999999999999E-3</v>
+      </c>
+      <c r="G963" s="5">
+        <v>7.4999999999999993E-5</v>
+      </c>
+      <c r="H963" s="5">
+        <v>256</v>
+      </c>
+      <c r="I963" s="5">
+        <v>1.089E-2</v>
+      </c>
+      <c r="J963" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="964" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A964" s="5">
+        <v>262144</v>
+      </c>
+      <c r="B964" s="5">
+        <v>1.0460000000000001E-3</v>
+      </c>
+      <c r="C964" s="5">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="D964" s="5">
+        <v>9.1280000000000007E-3</v>
+      </c>
+      <c r="E964" s="5">
+        <v>1.2799999999999999E-4</v>
+      </c>
+      <c r="F964" s="5">
+        <v>9.6900000000000003E-4</v>
+      </c>
+      <c r="G964" s="5">
+        <v>2.3599999999999999E-4</v>
+      </c>
+      <c r="H964" s="5">
+        <v>256</v>
+      </c>
+      <c r="I964" s="5">
+        <v>1.1143E-2</v>
+      </c>
+      <c r="J964" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="965" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A965" s="5">
+        <v>301124</v>
+      </c>
+      <c r="B965" s="5">
+        <v>2.3630000000000001E-3</v>
+      </c>
+      <c r="C965" s="5">
+        <v>9.59E-4</v>
+      </c>
+      <c r="D965" s="5">
+        <v>1.0636E-2</v>
+      </c>
+      <c r="E965" s="5">
+        <v>2.33E-4</v>
+      </c>
+      <c r="F965" s="5">
+        <v>1.1559999999999999E-3</v>
+      </c>
+      <c r="G965" s="5">
+        <v>9.5000000000000005E-5</v>
+      </c>
+      <c r="H965" s="5">
+        <v>256</v>
+      </c>
+      <c r="I965" s="5">
+        <v>1.4154999999999999E-2</v>
+      </c>
+      <c r="J965" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="966" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A966" s="5">
+        <v>345901</v>
+      </c>
+      <c r="B966" s="5">
+        <v>1.7849999999999999E-3</v>
+      </c>
+      <c r="C966" s="5">
+        <v>5.5999999999999999E-5</v>
+      </c>
+      <c r="D966" s="5">
+        <v>1.2315E-2</v>
+      </c>
+      <c r="E966" s="5">
+        <v>2.2100000000000001E-4</v>
+      </c>
+      <c r="F966" s="5">
+        <v>1.214E-3</v>
+      </c>
+      <c r="G966" s="5">
+        <v>1.47E-4</v>
+      </c>
+      <c r="H966" s="5">
+        <v>256</v>
+      </c>
+      <c r="I966" s="5">
+        <v>1.5313999999999999E-2</v>
+      </c>
+      <c r="J966" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="967" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A967" s="5">
+        <v>397336</v>
+      </c>
+      <c r="B967" s="5">
+        <v>1.7570000000000001E-3</v>
+      </c>
+      <c r="C967" s="5">
+        <v>2.5099999999999998E-4</v>
+      </c>
+      <c r="D967" s="5">
+        <v>1.4063000000000001E-2</v>
+      </c>
+      <c r="E967" s="5">
+        <v>9.7099999999999997E-4</v>
+      </c>
+      <c r="F967" s="5">
+        <v>1.3829999999999999E-3</v>
+      </c>
+      <c r="G967" s="5">
+        <v>1.02E-4</v>
+      </c>
+      <c r="H967" s="5">
+        <v>256</v>
+      </c>
+      <c r="I967" s="5">
+        <v>1.7204000000000001E-2</v>
+      </c>
+      <c r="J967" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="968" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A968" s="5">
+        <v>456419</v>
+      </c>
+      <c r="B968" s="5">
+        <v>2.049E-3</v>
+      </c>
+      <c r="C968" s="5">
+        <v>1.4100000000000001E-4</v>
+      </c>
+      <c r="D968" s="5">
+        <v>1.4586E-2</v>
+      </c>
+      <c r="E968" s="5">
+        <v>7.9199999999999995E-4</v>
+      </c>
+      <c r="F968" s="5">
+        <v>1.3990000000000001E-3</v>
+      </c>
+      <c r="G968" s="5">
+        <v>1.5200000000000001E-4</v>
+      </c>
+      <c r="H968" s="5">
+        <v>256</v>
+      </c>
+      <c r="I968" s="5">
+        <v>1.8034000000000001E-2</v>
+      </c>
+      <c r="J968" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="969" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A969" s="5">
+        <v>524288</v>
+      </c>
+      <c r="B969" s="5">
+        <v>1.7290000000000001E-3</v>
+      </c>
+      <c r="C969" s="5">
+        <v>8.8999999999999995E-5</v>
+      </c>
+      <c r="D969" s="5">
+        <v>1.6542000000000001E-2</v>
+      </c>
+      <c r="E969" s="5">
+        <v>2.6600000000000001E-4</v>
+      </c>
+      <c r="F969" s="5">
+        <v>1.57E-3</v>
+      </c>
+      <c r="G969" s="5">
+        <v>2.5900000000000001E-4</v>
+      </c>
+      <c r="H969" s="5">
+        <v>256</v>
+      </c>
+      <c r="I969" s="5">
+        <v>1.9841000000000001E-2</v>
+      </c>
+      <c r="J969" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="970" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A970" s="5">
+        <v>602248</v>
+      </c>
+      <c r="B970" s="5">
+        <v>3.2179999999999999E-3</v>
+      </c>
+      <c r="C970" s="5">
+        <v>1.3470000000000001E-3</v>
+      </c>
+      <c r="D970" s="5">
+        <v>1.8983E-2</v>
+      </c>
+      <c r="E970" s="5">
+        <v>4.9399999999999997E-4</v>
+      </c>
+      <c r="F970" s="5">
+        <v>1.7420000000000001E-3</v>
+      </c>
+      <c r="G970" s="5">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="H970" s="5">
+        <v>256</v>
+      </c>
+      <c r="I970" s="5">
+        <v>2.3942999999999999E-2</v>
+      </c>
+      <c r="J970" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="971" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A971" s="5">
+        <v>691802</v>
+      </c>
+      <c r="B971" s="5">
+        <v>2.5019999999999999E-3</v>
+      </c>
+      <c r="C971" s="5">
+        <v>2.2599999999999999E-4</v>
+      </c>
+      <c r="D971" s="5">
+        <v>2.1673000000000001E-2</v>
+      </c>
+      <c r="E971" s="5">
+        <v>4.64E-4</v>
+      </c>
+      <c r="F971" s="5">
+        <v>1.884E-3</v>
+      </c>
+      <c r="G971" s="5">
+        <v>2.5099999999999998E-4</v>
+      </c>
+      <c r="H971" s="5">
+        <v>256</v>
+      </c>
+      <c r="I971" s="5">
+        <v>2.6058999999999999E-2</v>
+      </c>
+      <c r="J971" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="972" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A972" s="5">
+        <v>794672</v>
+      </c>
+      <c r="B972" s="5">
+        <v>2.8270000000000001E-3</v>
+      </c>
+      <c r="C972" s="5">
+        <v>1.7899999999999999E-4</v>
+      </c>
+      <c r="D972" s="5">
+        <v>2.3290999999999999E-2</v>
+      </c>
+      <c r="E972" s="5">
+        <v>3.2400000000000001E-4</v>
+      </c>
+      <c r="F972" s="5">
+        <v>2.127E-3</v>
+      </c>
+      <c r="G972" s="5">
+        <v>4.1800000000000002E-4</v>
+      </c>
+      <c r="H972" s="5">
+        <v>256</v>
+      </c>
+      <c r="I972" s="5">
+        <v>2.8244999999999999E-2</v>
+      </c>
+      <c r="J972" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="973" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A973" s="5">
+        <v>912838</v>
+      </c>
+      <c r="B973" s="5">
+        <v>2.9759999999999999E-3</v>
+      </c>
+      <c r="C973" s="5">
+        <v>1.8900000000000001E-4</v>
+      </c>
+      <c r="D973" s="5">
+        <v>2.6235000000000001E-2</v>
+      </c>
+      <c r="E973" s="5">
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="F973" s="5">
+        <v>2.3770000000000002E-3</v>
+      </c>
+      <c r="G973" s="5">
+        <v>2.81E-4</v>
+      </c>
+      <c r="H973" s="5">
+        <v>256</v>
+      </c>
+      <c r="I973" s="5">
+        <v>3.1587999999999998E-2</v>
+      </c>
+      <c r="J973" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="974" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A974" s="5">
+        <v>1048576</v>
+      </c>
+      <c r="B974" s="5">
+        <v>2.8170000000000001E-3</v>
+      </c>
+      <c r="C974" s="5">
+        <v>2.4800000000000001E-4</v>
+      </c>
+      <c r="D974" s="5">
+        <v>3.0041999999999999E-2</v>
+      </c>
+      <c r="E974" s="5">
+        <v>3.2600000000000001E-4</v>
+      </c>
+      <c r="F974" s="5">
+        <v>2.4910000000000002E-3</v>
+      </c>
+      <c r="G974" s="5">
+        <v>5.0799999999999999E-4</v>
+      </c>
+      <c r="H974" s="5">
+        <v>256</v>
+      </c>
+      <c r="I974" s="5">
+        <v>3.5349999999999999E-2</v>
+      </c>
+      <c r="J974" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="975" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A975" s="5">
+        <v>1204497</v>
+      </c>
+      <c r="B975" s="5">
+        <v>3.6909999999999998E-3</v>
+      </c>
+      <c r="C975" s="5">
+        <v>2.5300000000000002E-4</v>
+      </c>
+      <c r="D975" s="5">
+        <v>3.4605999999999998E-2</v>
+      </c>
+      <c r="E975" s="5">
+        <v>6.4700000000000001E-4</v>
+      </c>
+      <c r="F975" s="5">
+        <v>3.0799999999999998E-3</v>
+      </c>
+      <c r="G975" s="5">
+        <v>8.8900000000000003E-4</v>
+      </c>
+      <c r="H975" s="5">
+        <v>256</v>
+      </c>
+      <c r="I975" s="5">
+        <v>4.1377999999999998E-2</v>
+      </c>
+      <c r="J975" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="976" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A976" s="5">
+        <v>1383604</v>
+      </c>
+      <c r="B976" s="5">
+        <v>4.1409999999999997E-3</v>
+      </c>
+      <c r="C976" s="5">
+        <v>1.0900000000000001E-4</v>
+      </c>
+      <c r="D976" s="5">
+        <v>3.9176999999999997E-2</v>
+      </c>
+      <c r="E976" s="5">
+        <v>4.08E-4</v>
+      </c>
+      <c r="F976" s="5">
+        <v>3.4680000000000002E-3</v>
+      </c>
+      <c r="G976" s="5">
+        <v>8.3199999999999995E-4</v>
+      </c>
+      <c r="H976" s="5">
+        <v>256</v>
+      </c>
+      <c r="I976" s="5">
+        <v>4.6786000000000001E-2</v>
+      </c>
+      <c r="J976" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="977" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A977" s="5">
+        <v>1589344</v>
+      </c>
+      <c r="B977" s="5">
+        <v>4.1770000000000002E-3</v>
+      </c>
+      <c r="C977" s="5">
+        <v>2.6699999999999998E-4</v>
+      </c>
+      <c r="D977" s="5">
+        <v>4.3898E-2</v>
+      </c>
+      <c r="E977" s="5">
+        <v>2.8200000000000002E-4</v>
+      </c>
+      <c r="F977" s="5">
+        <v>3.3579999999999999E-3</v>
+      </c>
+      <c r="G977" s="5">
+        <v>5.1900000000000004E-4</v>
+      </c>
+      <c r="H977" s="5">
+        <v>256</v>
+      </c>
+      <c r="I977" s="5">
+        <v>5.1434000000000001E-2</v>
+      </c>
+      <c r="J977" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="978" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A978" s="5">
+        <v>1825676</v>
+      </c>
+      <c r="B978" s="5">
+        <v>6.1830000000000001E-3</v>
+      </c>
+      <c r="C978" s="5">
+        <v>2.189E-3</v>
+      </c>
+      <c r="D978" s="5">
+        <v>5.0299000000000003E-2</v>
+      </c>
+      <c r="E978" s="5">
+        <v>9.3099999999999997E-4</v>
+      </c>
+      <c r="F978" s="5">
+        <v>3.9319999999999997E-3</v>
+      </c>
+      <c r="G978" s="5">
+        <v>4.4700000000000002E-4</v>
+      </c>
+      <c r="H978" s="5">
+        <v>256</v>
+      </c>
+      <c r="I978" s="5">
+        <v>6.0414000000000002E-2</v>
+      </c>
+      <c r="J978" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="979" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A979" s="5">
+        <v>2097152</v>
+      </c>
+      <c r="B979" s="5">
+        <v>4.6639999999999997E-3</v>
+      </c>
+      <c r="C979" s="5">
+        <v>2.5099999999999998E-4</v>
+      </c>
+      <c r="D979" s="5">
+        <v>5.6578000000000003E-2</v>
+      </c>
+      <c r="E979" s="5">
+        <v>2.4600000000000002E-4</v>
+      </c>
+      <c r="F979" s="5">
+        <v>4.3569999999999998E-3</v>
+      </c>
+      <c r="G979" s="5">
+        <v>6.5899999999999997E-4</v>
+      </c>
+      <c r="H979" s="5">
+        <v>256</v>
+      </c>
+      <c r="I979" s="5">
+        <v>6.5599000000000005E-2</v>
+      </c>
+      <c r="J979" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="980" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A980" s="5">
+        <v>2408995</v>
+      </c>
+      <c r="B980" s="5">
+        <v>6.1469999999999997E-3</v>
+      </c>
+      <c r="C980" s="5">
+        <v>1.4799999999999999E-4</v>
+      </c>
+      <c r="D980" s="5">
+        <v>6.4780000000000004E-2</v>
+      </c>
+      <c r="E980" s="5">
+        <v>4.7199999999999998E-4</v>
+      </c>
+      <c r="F980" s="5">
+        <v>5.0099999999999997E-3</v>
+      </c>
+      <c r="G980" s="5">
+        <v>7.5799999999999999E-4</v>
+      </c>
+      <c r="H980" s="5">
+        <v>256</v>
+      </c>
+      <c r="I980" s="5">
+        <v>7.5936000000000003E-2</v>
+      </c>
+      <c r="J980" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="981" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A981" s="5">
+        <v>2767208</v>
+      </c>
+      <c r="B981" s="5">
+        <v>6.5579999999999996E-3</v>
+      </c>
+      <c r="C981" s="5">
+        <v>4.0499999999999998E-4</v>
+      </c>
+      <c r="D981" s="5">
+        <v>7.3782E-2</v>
+      </c>
+      <c r="E981" s="5">
+        <v>5.6099999999999998E-4</v>
+      </c>
+      <c r="F981" s="5">
+        <v>5.5700000000000003E-3</v>
+      </c>
+      <c r="G981" s="5">
+        <v>9.2400000000000002E-4</v>
+      </c>
+      <c r="H981" s="5">
+        <v>256</v>
+      </c>
+      <c r="I981" s="5">
+        <v>8.591E-2</v>
+      </c>
+      <c r="J981" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="982" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A982" s="5">
+        <v>3178688</v>
+      </c>
+      <c r="B982" s="5">
+        <v>7.6099999999999996E-3</v>
+      </c>
+      <c r="C982" s="5">
+        <v>3.7500000000000001E-4</v>
+      </c>
+      <c r="D982" s="5">
+        <v>8.5591E-2</v>
+      </c>
+      <c r="E982" s="5">
+        <v>5.8799999999999998E-4</v>
+      </c>
+      <c r="F982" s="5">
+        <v>6.4219999999999998E-3</v>
+      </c>
+      <c r="G982" s="5">
+        <v>1.0989999999999999E-3</v>
+      </c>
+      <c r="H982" s="5">
+        <v>256</v>
+      </c>
+      <c r="I982" s="5">
+        <v>9.9623000000000003E-2</v>
+      </c>
+      <c r="J982" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="983" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A983" s="5">
+        <v>3651353</v>
+      </c>
+      <c r="B983" s="5">
+        <v>8.5710000000000005E-3</v>
+      </c>
+      <c r="C983" s="5">
+        <v>3.7500000000000001E-4</v>
+      </c>
+      <c r="D983" s="5">
+        <v>9.7182000000000004E-2</v>
+      </c>
+      <c r="E983" s="5">
+        <v>7.0500000000000001E-4</v>
+      </c>
+      <c r="F983" s="5">
+        <v>7.1659999999999996E-3</v>
+      </c>
+      <c r="G983" s="5">
+        <v>1.2390000000000001E-3</v>
+      </c>
+      <c r="H983" s="5">
+        <v>256</v>
+      </c>
+      <c r="I983" s="5">
+        <v>0.112918</v>
+      </c>
+      <c r="J983" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="984" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A984" s="5">
+        <v>4194304</v>
+      </c>
+      <c r="B984" s="5">
+        <v>8.5800000000000008E-3</v>
+      </c>
+      <c r="C984" s="5">
+        <v>5.5099999999999995E-4</v>
+      </c>
+      <c r="D984" s="5">
+        <v>0.111022</v>
+      </c>
+      <c r="E984" s="5">
+        <v>7.9500000000000003E-4</v>
+      </c>
+      <c r="F984" s="5">
+        <v>7.979E-3</v>
+      </c>
+      <c r="G984" s="5">
+        <v>1.3290000000000001E-3</v>
+      </c>
+      <c r="H984" s="5">
+        <v>256</v>
+      </c>
+      <c r="I984" s="5">
+        <v>0.127582</v>
+      </c>
+      <c r="J984" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="985" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A985" s="5">
+        <v>4817990</v>
+      </c>
+      <c r="B985" s="5">
+        <v>1.128E-2</v>
+      </c>
+      <c r="C985" s="5">
+        <v>4.26E-4</v>
+      </c>
+      <c r="D985" s="5">
+        <v>0.12754799999999999</v>
+      </c>
+      <c r="E985" s="5">
+        <v>7.4700000000000005E-4</v>
+      </c>
+      <c r="F985" s="5">
+        <v>9.6010000000000002E-3</v>
+      </c>
+      <c r="G985" s="5">
+        <v>2.0010000000000002E-3</v>
+      </c>
+      <c r="H985" s="5">
+        <v>256</v>
+      </c>
+      <c r="I985" s="5">
+        <v>0.14842900000000001</v>
+      </c>
+      <c r="J985" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="986" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A986" s="5">
+        <v>5534417</v>
+      </c>
+      <c r="B986" s="5">
+        <v>1.2695E-2</v>
+      </c>
+      <c r="C986" s="5">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="D986" s="5">
+        <v>0.144896</v>
+      </c>
+      <c r="E986" s="5">
+        <v>8.7799999999999998E-4</v>
+      </c>
+      <c r="F986" s="5">
+        <v>1.0577E-2</v>
+      </c>
+      <c r="G986" s="5">
+        <v>1.6869999999999999E-3</v>
+      </c>
+      <c r="H986" s="5">
+        <v>256</v>
+      </c>
+      <c r="I986" s="5">
+        <v>0.16816800000000001</v>
+      </c>
+      <c r="J986" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="987" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A987" s="5">
+        <v>6357376</v>
+      </c>
+      <c r="B987" s="5">
+        <v>1.4893999999999999E-2</v>
+      </c>
+      <c r="C987" s="5">
+        <v>4.8299999999999998E-4</v>
+      </c>
+      <c r="D987" s="5">
+        <v>0.16744899999999999</v>
+      </c>
+      <c r="E987" s="5">
+        <v>1.0480000000000001E-3</v>
+      </c>
+      <c r="F987" s="5">
+        <v>1.2689000000000001E-2</v>
+      </c>
+      <c r="G987" s="5">
+        <v>2.7729999999999999E-3</v>
+      </c>
+      <c r="H987" s="5">
+        <v>256</v>
+      </c>
+      <c r="I987" s="5">
+        <v>0.19503200000000001</v>
+      </c>
+      <c r="J987" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="988" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A988" s="5">
+        <v>7302707</v>
+      </c>
+      <c r="B988" s="5">
+        <v>1.6759E-2</v>
+      </c>
+      <c r="C988" s="5">
+        <v>6.8999999999999997E-4</v>
+      </c>
+      <c r="D988" s="5">
+        <v>0.191251</v>
+      </c>
+      <c r="E988" s="5">
+        <v>1.3339999999999999E-3</v>
+      </c>
+      <c r="F988" s="5">
+        <v>1.5285E-2</v>
+      </c>
+      <c r="G988" s="5">
+        <v>3.019E-3</v>
+      </c>
+      <c r="H988" s="5">
+        <v>256</v>
+      </c>
+      <c r="I988" s="5">
+        <v>0.22329399999999999</v>
+      </c>
+      <c r="J988" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="989" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A989" s="5">
+        <v>8388608</v>
+      </c>
+      <c r="B989" s="5">
+        <v>1.6479000000000001E-2</v>
+      </c>
+      <c r="C989" s="5">
+        <v>4.8500000000000003E-4</v>
+      </c>
+      <c r="D989" s="5">
+        <v>0.221883</v>
+      </c>
+      <c r="E989" s="5">
+        <v>1.18E-4</v>
+      </c>
+      <c r="F989" s="5">
+        <v>1.8459E-2</v>
+      </c>
+      <c r="G989" s="5">
+        <v>2.7009999999999998E-3</v>
+      </c>
+      <c r="H989" s="5">
+        <v>256</v>
+      </c>
+      <c r="I989" s="5">
+        <v>0.25682100000000002</v>
+      </c>
+      <c r="J989" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="990" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A990" s="5">
+        <v>9635980</v>
+      </c>
+      <c r="B990" s="5">
+        <v>2.1825000000000001E-2</v>
+      </c>
+      <c r="C990" s="5">
+        <v>4.0099999999999999E-4</v>
+      </c>
+      <c r="D990" s="5">
+        <v>0.25343500000000002</v>
+      </c>
+      <c r="E990" s="5">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="F990" s="5">
+        <v>2.1368000000000002E-2</v>
+      </c>
+      <c r="G990" s="5">
+        <v>3.6800000000000001E-3</v>
+      </c>
+      <c r="H990" s="5">
+        <v>256</v>
+      </c>
+      <c r="I990" s="5">
+        <v>0.29662899999999998</v>
+      </c>
+      <c r="J990" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="991" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A991" s="5">
+        <v>11068834</v>
+      </c>
+      <c r="B991" s="5">
+        <v>2.5152999999999998E-2</v>
+      </c>
+      <c r="C991" s="5">
+        <v>5.8900000000000001E-4</v>
+      </c>
+      <c r="D991" s="5">
+        <v>0.28972900000000001</v>
+      </c>
+      <c r="E991" s="5">
+        <v>2.7E-4</v>
+      </c>
+      <c r="F991" s="5">
+        <v>2.4261000000000001E-2</v>
+      </c>
+      <c r="G991" s="5">
+        <v>3.5109999999999998E-3</v>
+      </c>
+      <c r="H991" s="5">
+        <v>256</v>
+      </c>
+      <c r="I991" s="5">
+        <v>0.33914299999999997</v>
+      </c>
+      <c r="J991" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="992" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A992" s="5">
+        <v>12714752</v>
+      </c>
+      <c r="B992" s="5">
+        <v>2.8783E-2</v>
+      </c>
+      <c r="C992" s="5">
+        <v>8.3699999999999996E-4</v>
+      </c>
+      <c r="D992" s="5">
+        <v>0.33168599999999998</v>
+      </c>
+      <c r="E992" s="5">
+        <v>3.3799999999999998E-4</v>
+      </c>
+      <c r="F992" s="5">
+        <v>2.8480999999999999E-2</v>
+      </c>
+      <c r="G992" s="5">
+        <v>4.091E-3</v>
+      </c>
+      <c r="H992" s="5">
+        <v>256</v>
+      </c>
+      <c r="I992" s="5">
+        <v>0.38895099999999999</v>
+      </c>
+      <c r="J992" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="993" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A993" s="5">
+        <v>14605414</v>
+      </c>
+      <c r="B993" s="5">
+        <v>3.3205999999999999E-2</v>
+      </c>
+      <c r="C993" s="5">
+        <v>1.632E-3</v>
+      </c>
+      <c r="D993" s="5">
+        <v>0.38005100000000003</v>
+      </c>
+      <c r="E993" s="5">
+        <v>1.9100000000000001E-4</v>
+      </c>
+      <c r="F993" s="5">
+        <v>3.1801999999999997E-2</v>
+      </c>
+      <c r="G993" s="5">
+        <v>4.731E-3</v>
+      </c>
+      <c r="H993" s="5">
+        <v>256</v>
+      </c>
+      <c r="I993" s="5">
+        <v>0.44506000000000001</v>
+      </c>
+      <c r="J993" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="994" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A994" s="5">
+        <v>16777216</v>
+      </c>
+      <c r="B994" s="5">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="C994" s="5">
+        <v>6.7999999999999999E-5</v>
+      </c>
+      <c r="D994" s="5">
+        <v>0.44028099999999998</v>
+      </c>
+      <c r="E994" s="5">
+        <v>5.5999999999999999E-5</v>
+      </c>
+      <c r="F994" s="5">
+        <v>3.6541999999999998E-2</v>
+      </c>
+      <c r="G994" s="5">
+        <v>5.4419999999999998E-3</v>
+      </c>
+      <c r="H994" s="5">
+        <v>256</v>
+      </c>
+      <c r="I994" s="5">
+        <v>0.51392400000000005</v>
+      </c>
+      <c r="J994" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="995" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A995" s="5">
+        <v>19271960</v>
+      </c>
+      <c r="B995" s="5">
+        <v>4.5603999999999999E-2</v>
+      </c>
+      <c r="C995" s="5">
+        <v>4.0299999999999998E-4</v>
+      </c>
+      <c r="D995" s="5">
+        <v>0.50109300000000001</v>
+      </c>
+      <c r="E995" s="5">
+        <v>1.6100000000000001E-4</v>
+      </c>
+      <c r="F995" s="5">
+        <v>4.1419999999999998E-2</v>
+      </c>
+      <c r="G995" s="5">
+        <v>5.7279999999999996E-3</v>
+      </c>
+      <c r="H995" s="5">
+        <v>256</v>
+      </c>
+      <c r="I995" s="5">
+        <v>0.588117</v>
+      </c>
+      <c r="J995" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="996" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A996" s="5">
+        <v>22137669</v>
+      </c>
+      <c r="B996" s="5">
+        <v>5.1806999999999999E-2</v>
+      </c>
+      <c r="C996" s="5">
+        <v>2.6499999999999999E-4</v>
+      </c>
+      <c r="D996" s="5">
+        <v>0.574855</v>
+      </c>
+      <c r="E996" s="5">
+        <v>4.86E-4</v>
+      </c>
+      <c r="F996" s="5">
+        <v>4.7238000000000002E-2</v>
+      </c>
+      <c r="G996" s="5">
+        <v>6.3790000000000001E-3</v>
+      </c>
+      <c r="H996" s="5">
+        <v>256</v>
+      </c>
+      <c r="I996" s="5">
+        <v>0.67390000000000005</v>
+      </c>
+      <c r="J996" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="997" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A997" s="5">
+        <v>25429504</v>
+      </c>
+      <c r="B997" s="5">
+        <v>6.0198000000000002E-2</v>
+      </c>
+      <c r="C997" s="5">
+        <v>3.2699999999999998E-4</v>
+      </c>
+      <c r="D997" s="5">
+        <v>0.66328600000000004</v>
+      </c>
+      <c r="E997" s="5">
+        <v>2.8800000000000001E-4</v>
+      </c>
+      <c r="F997" s="5">
+        <v>5.4254999999999998E-2</v>
+      </c>
+      <c r="G997" s="5">
+        <v>7.2090000000000001E-3</v>
+      </c>
+      <c r="H997" s="5">
+        <v>256</v>
+      </c>
+      <c r="I997" s="5">
+        <v>0.77773899999999996</v>
+      </c>
+      <c r="J997" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="998" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A998" s="5">
+        <v>29210829</v>
+      </c>
+      <c r="B998" s="5">
+        <v>6.9157999999999997E-2</v>
+      </c>
+      <c r="C998" s="5">
+        <v>2.7599999999999999E-4</v>
+      </c>
+      <c r="D998" s="5">
+        <v>0.76040399999999997</v>
+      </c>
+      <c r="E998" s="5">
+        <v>8.2700000000000004E-4</v>
+      </c>
+      <c r="F998" s="5">
+        <v>6.1886999999999998E-2</v>
+      </c>
+      <c r="G998" s="5">
+        <v>8.5039999999999994E-3</v>
+      </c>
+      <c r="H998" s="5">
+        <v>256</v>
+      </c>
+      <c r="I998" s="5">
+        <v>0.89144900000000005</v>
+      </c>
+      <c r="J998" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="999" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A999" s="5">
+        <v>33554432</v>
+      </c>
+      <c r="B999" s="5">
+        <v>7.4732000000000007E-2</v>
+      </c>
+      <c r="C999" s="5">
+        <v>1.36E-4</v>
+      </c>
+      <c r="D999" s="5">
+        <v>0.87198699999999996</v>
+      </c>
+      <c r="E999" s="5">
+        <v>2.7179999999999999E-3</v>
+      </c>
+      <c r="F999" s="5">
+        <v>7.2397000000000003E-2</v>
+      </c>
+      <c r="G999" s="5">
+        <v>9.325E-3</v>
+      </c>
+      <c r="H999" s="5">
+        <v>256</v>
+      </c>
+      <c r="I999" s="5">
+        <v>1.0191159999999999</v>
+      </c>
+      <c r="J999" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1000" s="5">
+        <v>38543920</v>
+      </c>
+      <c r="B1000" s="5">
+        <v>9.1037999999999994E-2</v>
+      </c>
+      <c r="C1000" s="5">
+        <v>7.7999999999999999E-5</v>
+      </c>
+      <c r="D1000" s="5">
+        <v>1.0026219999999999</v>
+      </c>
+      <c r="E1000" s="5">
+        <v>1.041E-3</v>
+      </c>
+      <c r="F1000" s="5">
+        <v>8.0154000000000003E-2</v>
+      </c>
+      <c r="G1000" s="5">
+        <v>1.0597000000000001E-2</v>
+      </c>
+      <c r="H1000" s="5">
+        <v>256</v>
+      </c>
+      <c r="I1000" s="5">
+        <v>1.1738139999999999</v>
+      </c>
+      <c r="J1000" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1001" s="5">
+        <v>44275338</v>
+      </c>
+      <c r="B1001" s="5">
+        <v>0.104573</v>
+      </c>
+      <c r="C1001" s="5">
+        <v>3.1100000000000002E-4</v>
+      </c>
+      <c r="D1001" s="5">
+        <v>1.1494629999999999</v>
+      </c>
+      <c r="E1001" s="5">
+        <v>2.9500000000000001E-4</v>
+      </c>
+      <c r="F1001" s="5">
+        <v>9.3187999999999993E-2</v>
+      </c>
+      <c r="G1001" s="5">
+        <v>1.2533000000000001E-2</v>
+      </c>
+      <c r="H1001" s="5">
+        <v>256</v>
+      </c>
+      <c r="I1001" s="5">
+        <v>1.347224</v>
+      </c>
+      <c r="J1001" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1002" s="5">
+        <v>50859008</v>
+      </c>
+      <c r="B1002" s="5">
+        <v>0.119936</v>
+      </c>
+      <c r="C1002" s="5">
+        <v>6.6000000000000005E-5</v>
+      </c>
+      <c r="D1002" s="5">
+        <v>1.3157160000000001</v>
+      </c>
+      <c r="E1002" s="5">
+        <v>1.219E-3</v>
+      </c>
+      <c r="F1002" s="5">
+        <v>0.106378</v>
+      </c>
+      <c r="G1002" s="5">
+        <v>1.4120000000000001E-2</v>
+      </c>
+      <c r="H1002" s="5">
+        <v>256</v>
+      </c>
+      <c r="I1002" s="5">
+        <v>1.54203</v>
+      </c>
+      <c r="J1002" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1003" s="5">
+        <v>58421659</v>
+      </c>
+      <c r="B1003" s="5">
+        <v>0.137484</v>
+      </c>
+      <c r="C1003" s="5">
+        <v>5.6999999999999998E-4</v>
+      </c>
+      <c r="D1003" s="5">
+        <v>1.5097020000000001</v>
+      </c>
+      <c r="E1003" s="5">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="F1003" s="5">
+        <v>0.120557</v>
+      </c>
+      <c r="G1003" s="5">
+        <v>1.5499000000000001E-2</v>
+      </c>
+      <c r="H1003" s="5">
+        <v>256</v>
+      </c>
+      <c r="I1003" s="5">
+        <v>1.7677419999999999</v>
+      </c>
+      <c r="J1003" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1004" s="5">
+        <v>67108864</v>
+      </c>
+      <c r="B1004" s="5">
+        <v>0.15456400000000001</v>
+      </c>
+      <c r="C1004" s="5">
+        <v>4.4000000000000002E-4</v>
+      </c>
+      <c r="D1004" s="5">
+        <v>1.740704</v>
+      </c>
+      <c r="E1004" s="5">
+        <v>1.057E-3</v>
+      </c>
+      <c r="F1004" s="5">
+        <v>0.13999600000000001</v>
+      </c>
+      <c r="G1004" s="5">
+        <v>1.7998E-2</v>
+      </c>
+      <c r="H1004" s="5">
+        <v>256</v>
+      </c>
+      <c r="I1004" s="5">
+        <v>2.0352649999999999</v>
+      </c>
+      <c r="J1004" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1005" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1005" s="5">
+        <v>1.75E-4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>